<commit_message>
More editing. Code is working as you would like with the classes etc. There is a problem with the interpretation of the parameters L and Lcoup.
</commit_message>
<xml_diff>
--- a/ORR_Filter/ORR_Filter/Plots.xlsx
+++ b/ORR_Filter/ORR_Filter/Plots.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -105,7 +105,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,607 +808,607 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="431"/>
                 <c:pt idx="0">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99995939199999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99999976899999998</c:v>
+                  <c:v>0.99993383520000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99999976840000004</c:v>
+                  <c:v>0.77410293770000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99992241299999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99999916209999995</c:v>
+                  <c:v>0.99996121770000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99994441359999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.99999976859999995</c:v>
+                  <c:v>0.99974407379999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99999976899999998</c:v>
+                  <c:v>0.99736309430000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99986849560000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.99999975419999998</c:v>
+                  <c:v>0.99994212100000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99995769850000005</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.99999976660000001</c:v>
+                  <c:v>0.9999612859</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99996074489999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.9999590236</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.99999976739999996</c:v>
+                  <c:v>0.9999579475</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.9999584064</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.99999970120000004</c:v>
+                  <c:v>0.99996002679999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99996134579999996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.99999976850000005</c:v>
+                  <c:v>0.99996006370000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.99999976909999999</c:v>
+                  <c:v>0.99995157499999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.9999175683</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.9999997638</c:v>
+                  <c:v>0.99964708719999995</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99818933210000005</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.99999975900000004</c:v>
+                  <c:v>0.99990579670000002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99995857070000005</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.99999976879999997</c:v>
+                  <c:v>0.99995400759999997</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.99999976889999997</c:v>
+                  <c:v>0.99976291019999997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99973956959999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.99999976209999997</c:v>
+                  <c:v>0.99995762479999994</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99994062409999995</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.99999975860000001</c:v>
+                  <c:v>0.99132990649999997</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99995297490000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.99999976869999996</c:v>
+                  <c:v>0.99993490340000002</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.99999976899999998</c:v>
+                  <c:v>0.99960724459999994</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99996138950000002</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.99999976580000005</c:v>
+                  <c:v>0.99932605240000005</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99995355500000005</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.99999968569999997</c:v>
+                  <c:v>0.99985670550000005</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99994336949999996</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.99999976779999999</c:v>
+                  <c:v>0.99987720889999998</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99994859970000005</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.9999997692</c:v>
+                  <c:v>0.99973471020000004</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.99999976830000004</c:v>
+                  <c:v>0.99995991139999996</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99117504190000005</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.99999975539999997</c:v>
+                  <c:v>0.9999550076</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.9999208758</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.99999975669999996</c:v>
+                  <c:v>0.99967705569999998</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99996042439999999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.99999976830000004</c:v>
+                  <c:v>0.99991328430000004</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.999102763</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.9999997692</c:v>
+                  <c:v>0.99995060499999999</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.99999976830000004</c:v>
+                  <c:v>0.99995700970000001</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99982867379999996</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.99999976049999995</c:v>
+                  <c:v>0.99899775499999999</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99992869419999997</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.99999972339999998</c:v>
+                  <c:v>0.99996014720000004</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99995694830000004</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.99999976710000005</c:v>
+                  <c:v>0.9999248758</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99976240149999995</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.99999976889999997</c:v>
+                  <c:v>0.99534515270000001</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.99999976899999998</c:v>
+                  <c:v>0.99869562150000002</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99971262390000004</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.99999976769999999</c:v>
+                  <c:v>0.99984201130000006</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99987834060000003</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.99999975640000005</c:v>
+                  <c:v>0.99988547520000004</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99987161560000004</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.99999970380000003</c:v>
+                  <c:v>0.99981986720000005</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99961508239999997</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.99999976589999995</c:v>
+                  <c:v>0.99638030180000003</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99874250369999995</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.99999976850000005</c:v>
+                  <c:v>0.99984043690000002</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99993818229999998</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.9999997692</c:v>
+                  <c:v>0.99995973400000004</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.99999976879999997</c:v>
+                  <c:v>0.99995744480000004</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99990420369999999</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.99999976739999996</c:v>
+                  <c:v>0.98686493220000004</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99989175109999995</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.99999976040000005</c:v>
+                  <c:v>0.99996009350000004</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99994124350000002</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.99999707230000001</c:v>
+                  <c:v>0.99352246980000003</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99993166779999998</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.99999975640000005</c:v>
+                  <c:v>0.99995863200000001</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99944949370000002</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.9999997665</c:v>
+                  <c:v>0.99992962110000005</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99995377259999996</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.99999976830000004</c:v>
+                  <c:v>0.99066593830000005</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99995919779999998</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.99999976899999998</c:v>
+                  <c:v>0.99981659590000005</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.99999976909999999</c:v>
+                  <c:v>0.99993839920000005</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.9999997692</c:v>
+                  <c:v>0.99992293809999999</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.99999976869999996</c:v>
+                  <c:v>0.99991087670000001</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99993363189999995</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.99999976800000001</c:v>
+                  <c:v>0.99991710739999995</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99991143790000003</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.99999976629999998</c:v>
+                  <c:v>0.99994621019999996</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99966765909999999</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.99999976130000001</c:v>
+                  <c:v>0.99996117100000004</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99938248399999996</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.999999733</c:v>
+                  <c:v>0.99994051989999999</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99995017320000001</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.34018122779999999</c:v>
+                  <c:v>0.57150331489999995</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99994686870000005</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.99999972640000001</c:v>
+                  <c:v>0.99995406050000002</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99937763820000003</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>0.99999975799999996</c:v>
+                  <c:v>0.99987996980000005</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99996023020000002</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0.99999976410000002</c:v>
+                  <c:v>0.99994566080000002</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99959974200000001</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>0.99999976629999998</c:v>
+                  <c:v>0.99960430280000001</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99993653689999995</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>0.99999976729999995</c:v>
+                  <c:v>0.99996044139999996</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.9999574309</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>0.9999997679</c:v>
+                  <c:v>0.99993150590000002</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99982656749999999</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>0.99999976820000003</c:v>
+                  <c:v>0.99888925210000001</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99029413249999998</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>0.99999976850000005</c:v>
+                  <c:v>0.99940634719999999</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99974394109999998</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>0.99999976859999995</c:v>
+                  <c:v>0.99982276569999995</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99984274829999997</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>0.99999976869999996</c:v>
+                  <c:v>0.99983039819999997</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99977044449999997</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>0.99999976879999997</c:v>
+                  <c:v>0.99954047619999997</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99691584840000003</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>0.99999976879999997</c:v>
+                  <c:v>0.9974927039</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99976055789999996</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>0.99999976879999997</c:v>
+                  <c:v>0.99991779179999996</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99995362300000001</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>0.99999976869999996</c:v>
+                  <c:v>0.9999613678</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.9999485186</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>0.99999976869999996</c:v>
+                  <c:v>0.99982834939999998</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99699477079999999</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>0.99999976859999995</c:v>
+                  <c:v>0.99992075130000002</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99996108459999999</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>0.99999976840000004</c:v>
+                  <c:v>0.99993692850000004</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99433581999999998</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>0.99999976820000003</c:v>
+                  <c:v>0.99992301920000004</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99996069499999996</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>0.99999976779999999</c:v>
+                  <c:v>0.99980952609999996</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99986259430000002</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>0.99999976719999994</c:v>
+                  <c:v>0.99996124710000001</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99972547810000001</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>0.99999976609999996</c:v>
+                  <c:v>0.9999244008</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99995229809999997</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>0.9999997638</c:v>
+                  <c:v>0.99854328469999998</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99996116719999995</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>0.99999975730000001</c:v>
+                  <c:v>0.99943753319999995</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99995449030000005</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>0.99999972370000001</c:v>
+                  <c:v>0.99982462729999999</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99994867939999998</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>0.34018122779999999</c:v>
+                  <c:v>0.99983686230000002</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99995286159999996</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>0.9999997303</c:v>
+                  <c:v>0.99962112759999999</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99996043229999998</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>0.99999976069999996</c:v>
+                  <c:v>0.98980068929999998</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99995693860000001</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>0.99999976599999996</c:v>
+                  <c:v>0.99989390909999998</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99986242280000004</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>0.99999976779999999</c:v>
+                  <c:v>0.99996063859999995</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99963125959999999</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>0.99999976859999995</c:v>
+                  <c:v>0.99991250210000004</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99996041719999995</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>0.99999976909999999</c:v>
+                  <c:v>0.99980398339999998</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>0.99999976909999999</c:v>
+                  <c:v>0.99979377729999996</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99995847090000001</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>0.99999976859999995</c:v>
+                  <c:v>0.99994779050000004</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99948660180000004</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>0.99999976749999997</c:v>
+                  <c:v>0.99978001699999997</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99995094679999996</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>0.99999976329999996</c:v>
+                  <c:v>0.9999607439</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99993521490000004</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>0.99999970140000005</c:v>
+                  <c:v>0.99970333050000004</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99585628079999999</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>0.99999973070000003</c:v>
+                  <c:v>0.99983951029999996</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99993497539999998</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>0.99999976499999998</c:v>
+                  <c:v>0.99995548010000002</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99996097589999999</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>0.99999976810000002</c:v>
+                  <c:v>0.99996084689999998</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.9999579072</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>0.99999976899999998</c:v>
+                  <c:v>0.99995378690000003</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>0.99999976909999999</c:v>
+                  <c:v>0.99995009619999997</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99994836330000003</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>0.99999976830000004</c:v>
+                  <c:v>0.99994936420000002</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99995263909999998</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>0.99999976530000001</c:v>
+                  <c:v>0.99995679429999995</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99996021329999996</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>0.99999969249999998</c:v>
+                  <c:v>0.99996134759999999</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99995802280000001</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>0.99999975399999996</c:v>
+                  <c:v>0.99994422189999999</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.99989001970000002</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>0.99999976729999995</c:v>
+                  <c:v>0.9993052067</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>0.99999976940000002</c:v>
+                  <c:v>0.99907871859999997</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>0.99999976889999997</c:v>
+                  <c:v>0.99990611190000001</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>0.99999976909999999</c:v>
+                  <c:v>0.99995658350000005</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>0.99999976930000001</c:v>
+                  <c:v>0.99995904459999996</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>0.99999976810000002</c:v>
+                  <c:v>0.99990713600000003</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.94071497439999996</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>0.99999976140000002</c:v>
+                  <c:v>0.99990694270000002</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>0.99999976960000003</c:v>
+                  <c:v>0.99996097149999996</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>0.99999961410000004</c:v>
+                  <c:v>0.99993301329999995</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>0.99999976950000002</c:v>
+                  <c:v>0.57150331489999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2054,607 +2054,607 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="431"/>
                 <c:pt idx="0">
-                  <c:v>2.3053978730000001E-7</c:v>
+                  <c:v>4.0608006929999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.30963743E-7</c:v>
+                  <c:v>6.6164787730000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.316451382E-7</c:v>
+                  <c:v>0.22589706230000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3046828349999999E-7</c:v>
+                  <c:v>7.7586964230000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3788037630000003E-7</c:v>
+                  <c:v>3.8782293189999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3048234520000001E-7</c:v>
+                  <c:v>5.5586431730000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3143516839999999E-7</c:v>
+                  <c:v>2.5592619869999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3103116439999999E-7</c:v>
+                  <c:v>2.6369057179999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3053394060000001E-7</c:v>
+                  <c:v>1.3150441149999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4581589839999999E-7</c:v>
+                  <c:v>5.7879000499999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3044260410000001E-7</c:v>
+                  <c:v>4.2301520619999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3343634699999999E-7</c:v>
+                  <c:v>3.871409744E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.306685992E-7</c:v>
+                  <c:v>3.9255064039999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.3072904550000001E-7</c:v>
+                  <c:v>4.0976381100000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3255943160000001E-7</c:v>
+                  <c:v>4.2052474260000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.304514027E-7</c:v>
+                  <c:v>4.1593563580000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.988315564E-7</c:v>
+                  <c:v>3.9973183370000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3048932099999999E-7</c:v>
+                  <c:v>3.8654200430000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.314768143E-7</c:v>
+                  <c:v>3.9936312229999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.3094197890000001E-7</c:v>
+                  <c:v>4.8425036780000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.3057452610000001E-7</c:v>
+                  <c:v>8.2431701340000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.361711794E-7</c:v>
+                  <c:v>3.5291283470000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.3043865120000001E-7</c:v>
+                  <c:v>1.8106678860000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.410032331E-7</c:v>
+                  <c:v>9.4203291190000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.305315087E-7</c:v>
+                  <c:v>4.1429328869999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.311614609E-7</c:v>
+                  <c:v>4.5992363829999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3110017669999999E-7</c:v>
+                  <c:v>2.370898474E-4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.3054519800000001E-7</c:v>
+                  <c:v>2.6043040009999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3790932170000001E-7</c:v>
+                  <c:v>4.2375247829999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3043832259999999E-7</c:v>
+                  <c:v>5.9375938280000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.4135524049999998E-7</c:v>
+                  <c:v>8.6700935429999994E-3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.30521684E-7</c:v>
+                  <c:v>4.7025090339999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3128686930000001E-7</c:v>
+                  <c:v>6.5096647460000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3096623660000001E-7</c:v>
+                  <c:v>3.9275537929999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.3059022850000001E-7</c:v>
+                  <c:v>3.8610503850000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.342124193E-7</c:v>
+                  <c:v>6.7394757440000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.3044530080000001E-7</c:v>
+                  <c:v>4.6445001069999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.1432991170000002E-7</c:v>
+                  <c:v>1.4329449630000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.304713973E-7</c:v>
+                  <c:v>5.6630522490000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.321979995E-7</c:v>
+                  <c:v>1.227910508E-4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.306961597E-7</c:v>
+                  <c:v>5.1400267119999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.3078498720000001E-7</c:v>
+                  <c:v>2.6528976839999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.3165595759999999E-7</c:v>
+                  <c:v>4.0088576590000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.304987392E-7</c:v>
+                  <c:v>8.8249581389999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.446112259E-7</c:v>
+                  <c:v>4.499235362E-5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.3043818249999999E-7</c:v>
+                  <c:v>7.9124231799999995E-5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.433029305E-7</c:v>
+                  <c:v>3.229442893E-4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.304991805E-7</c:v>
+                  <c:v>3.9575577929999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.317181291E-7</c:v>
+                  <c:v>8.6715669049999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.307480407E-7</c:v>
+                  <c:v>8.9723696549999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.3075430590000001E-7</c:v>
+                  <c:v>4.9394998649999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.316625287E-7</c:v>
+                  <c:v>4.2990252659999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.3050664829999999E-7</c:v>
+                  <c:v>1.7132619090000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.3952032499999998E-7</c:v>
+                  <c:v>1.002244969E-3</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.3043966410000001E-7</c:v>
+                  <c:v>7.1305785420000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.7655972950000001E-7</c:v>
+                  <c:v>3.9852756430000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.3046680750000001E-7</c:v>
+                  <c:v>4.3051694829999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.3287505670000001E-7</c:v>
+                  <c:v>7.5124235449999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.3060247460000001E-7</c:v>
+                  <c:v>2.3759845809999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.3106718260000001E-7</c:v>
+                  <c:v>4.6548472999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2.309817621E-7</c:v>
+                  <c:v>1.3043784869999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2.3063482260000001E-7</c:v>
+                  <c:v>2.8737612249999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2.323039863E-7</c:v>
+                  <c:v>1.579886857E-4</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2.3048456370000001E-7</c:v>
+                  <c:v>1.216594168E-4</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2.4363247789999999E-7</c:v>
+                  <c:v>1.1452476710000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>2.3043919120000001E-7</c:v>
+                  <c:v>1.28384413E-4</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>2.9622215670000002E-7</c:v>
+                  <c:v>1.8013280010000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>2.304578414E-7</c:v>
+                  <c:v>3.8491758929999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2.3408075370000001E-7</c:v>
+                  <c:v>3.6196981719999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2.3054389349999999E-7</c:v>
+                  <c:v>1.257496343E-3</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2.314723027E-7</c:v>
+                  <c:v>1.5956313800000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>2.3074298290000001E-7</c:v>
+                  <c:v>6.1817680940000005E-5</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>2.3083365650000001E-7</c:v>
+                  <c:v>4.0265960210000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>2.3120832490000001E-7</c:v>
+                  <c:v>4.2555186469999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>2.3059204749999999E-7</c:v>
+                  <c:v>9.5796267729999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>2.325662322E-7</c:v>
+                  <c:v>1.313506777E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>2.3048605309999999E-7</c:v>
+                  <c:v>1.0824894640000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>2.396416645E-7</c:v>
+                  <c:v>3.9906541720000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>2.3044377779999999E-7</c:v>
+                  <c:v>5.8756486689999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>2.9277270639999999E-6</c:v>
+                  <c:v>6.4775301570000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>2.3044134370000001E-7</c:v>
+                  <c:v>6.8332177250000006E-5</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2.4362467690000001E-7</c:v>
+                  <c:v>4.1367956700000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2.3047264120000001E-7</c:v>
+                  <c:v>5.5050625099999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>2.334504275E-7</c:v>
+                  <c:v>7.0378924260000006E-5</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>2.305420049E-7</c:v>
+                  <c:v>4.6227376790000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>2.3166058569999999E-7</c:v>
+                  <c:v>9.3340617389999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>2.3066497619999999E-7</c:v>
+                  <c:v>4.080221217E-5</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2.3104181430000001E-7</c:v>
+                  <c:v>1.8340414600000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2.3087633899999999E-7</c:v>
+                  <c:v>6.1600821439999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>2.307590936E-7</c:v>
+                  <c:v>7.7061856030000004E-5</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2.312536772E-7</c:v>
+                  <c:v>8.9123311180000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2.306099544E-7</c:v>
+                  <c:v>6.6368127200000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>2.3198943339999999E-7</c:v>
+                  <c:v>8.2892625919999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2.305254543E-7</c:v>
+                  <c:v>8.8562148310000006E-5</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>2.3366072889999999E-7</c:v>
+                  <c:v>5.378976086E-5</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>2.3047688809999999E-7</c:v>
+                  <c:v>3.3234086359999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2.3866597280000002E-7</c:v>
+                  <c:v>3.8829012670000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.304505959E-7</c:v>
+                  <c:v>6.1751595630000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2.6698977380000002E-7</c:v>
+                  <c:v>5.94801035E-5</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2.304394234E-7</c:v>
+                  <c:v>4.9826769390000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.65981877219999996</c:v>
+                  <c:v>0.4284966851</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>2.3043932369999999E-7</c:v>
+                  <c:v>5.3131317670000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>2.7361736700000002E-7</c:v>
+                  <c:v>4.593946118E-5</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>2.3044782380000001E-7</c:v>
+                  <c:v>6.2236176299999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>2.4201199670000001E-7</c:v>
+                  <c:v>1.200302451E-4</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>2.3046325080000001E-7</c:v>
+                  <c:v>3.9769848569999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>2.359271893E-7</c:v>
+                  <c:v>5.4339213339999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>2.304842972E-7</c:v>
+                  <c:v>4.0025799429999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>2.3372676820000001E-7</c:v>
+                  <c:v>3.9569715030000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>2.305097523E-7</c:v>
+                  <c:v>6.3463143110000005E-5</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>2.3268193140000001E-7</c:v>
+                  <c:v>3.9558598330000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>2.3053832749999999E-7</c:v>
+                  <c:v>4.2569108459999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>2.321052871E-7</c:v>
+                  <c:v>6.8494124189999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>2.3056855099999999E-7</c:v>
+                  <c:v>1.7343253359999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>2.3175688600000001E-7</c:v>
+                  <c:v>1.1107479070000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>2.3059872989999999E-7</c:v>
+                  <c:v>9.7058675489999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>2.315349503E-7</c:v>
+                  <c:v>5.9365283949999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>2.3062698709999999E-7</c:v>
+                  <c:v>2.5605885190000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>2.313904414E-7</c:v>
+                  <c:v>1.7723428050000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>2.3065137640000001E-7</c:v>
+                  <c:v>1.572517208E-4</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>2.312977023E-7</c:v>
+                  <c:v>1.6960184250000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>2.3067006699999999E-7</c:v>
+                  <c:v>2.2955551850000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>2.312427682E-7</c:v>
+                  <c:v>4.595237992E-4</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>2.3068156319999999E-7</c:v>
+                  <c:v>3.0841516299999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>2.3121824329999999E-7</c:v>
+                  <c:v>2.5072960509999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>2.306849152E-7</c:v>
+                  <c:v>2.3944214650000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>2.3122098910000001E-7</c:v>
+                  <c:v>8.22081809E-5</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>2.3067986379999999E-7</c:v>
+                  <c:v>4.637698821E-5</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>2.3125122689999999E-7</c:v>
+                  <c:v>3.8632215389999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>2.3066687749999999E-7</c:v>
+                  <c:v>5.1481385129999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>2.3131258199999999E-7</c:v>
+                  <c:v>1.7165058499999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>2.306470744E-7</c:v>
+                  <c:v>3.0052292049999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>2.31413085E-7</c:v>
+                  <c:v>7.9248652110000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>2.3062204879999999E-7</c:v>
+                  <c:v>3.8915431740000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>2.3156765470000001E-7</c:v>
+                  <c:v>6.3071473739999994E-5</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>2.3059365160000001E-7</c:v>
+                  <c:v>5.6641800080000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>2.31803548E-7</c:v>
+                  <c:v>7.6980817890000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>2.3056377920000001E-7</c:v>
+                  <c:v>3.9304988819999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>2.3217277569999999E-7</c:v>
+                  <c:v>1.904738684E-4</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>2.305342102E-7</c:v>
+                  <c:v>1.3740569449999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>2.3278328089999999E-7</c:v>
+                  <c:v>3.8752937859999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>2.305065134E-7</c:v>
+                  <c:v>2.7452194129999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>2.338897243E-7</c:v>
+                  <c:v>7.5599163030000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>2.3048203070000001E-7</c:v>
+                  <c:v>4.770191941E-5</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>2.3622238899999999E-7</c:v>
+                  <c:v>1.4567152800000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>2.304619231E-7</c:v>
+                  <c:v>3.8832843970000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>2.4268385559999998E-7</c:v>
+                  <c:v>5.6246680240000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>2.3044727499999999E-7</c:v>
+                  <c:v>4.5509734060000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>2.7632079480000001E-7</c:v>
+                  <c:v>1.7537272560000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>2.304392532E-7</c:v>
+                  <c:v>5.1320573069999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>0.65981877219999996</c:v>
+                  <c:v>1.6313768640000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>2.304393406E-7</c:v>
+                  <c:v>4.7138380119999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>2.6969389080000002E-7</c:v>
+                  <c:v>3.7887237270000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>2.304497005E-7</c:v>
+                  <c:v>3.9567738049999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>2.393391829E-7</c:v>
+                  <c:v>1.01993107E-2</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>2.3047380159999999E-7</c:v>
+                  <c:v>4.3061404710000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>2.3395788410000001E-7</c:v>
+                  <c:v>1.060908947E-4</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>2.3051760669999999E-7</c:v>
+                  <c:v>1.3757724960000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>2.321548503E-7</c:v>
+                  <c:v>3.936141365E-5</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>2.305920839E-7</c:v>
+                  <c:v>3.687403763E-4</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>2.3135783340000001E-7</c:v>
+                  <c:v>8.7497919250000006E-5</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>2.3071913899999999E-7</c:v>
+                  <c:v>3.9582835309999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>2.309467264E-7</c:v>
+                  <c:v>1.9601663139999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>2.3094770370000001E-7</c:v>
+                  <c:v>2.0622267300000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>2.30714216E-7</c:v>
+                  <c:v>4.1529124099999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>2.314063736E-7</c:v>
+                  <c:v>5.2209521510000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>2.30576273E-7</c:v>
+                  <c:v>5.133981914E-4</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>2.325320109E-7</c:v>
+                  <c:v>2.199829933E-4</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>2.3049462119999999E-7</c:v>
+                  <c:v>4.9053235049999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>2.367156594E-7</c:v>
+                  <c:v>3.9256098470000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>2.304510941E-7</c:v>
+                  <c:v>6.4785090479999995E-5</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>2.986279805E-7</c:v>
+                  <c:v>2.9666945419999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>2.3043823260000001E-7</c:v>
+                  <c:v>4.1437191959999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>2.6925280840000001E-7</c:v>
+                  <c:v>1.6048974050000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>2.3045646970000001E-7</c:v>
+                  <c:v>6.5024635949999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>2.3504335219999999E-7</c:v>
+                  <c:v>4.4519864950000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>2.305159188E-7</c:v>
+                  <c:v>3.9024149390000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>2.319061618E-7</c:v>
+                  <c:v>3.915310307E-5</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>2.306461141E-7</c:v>
+                  <c:v>4.2092825300000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>2.310353532E-7</c:v>
+                  <c:v>4.62130988E-5</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>2.309318941E-7</c:v>
+                  <c:v>4.9903782309999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>2.306880463E-7</c:v>
+                  <c:v>5.1636682540000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>2.316790041E-7</c:v>
+                  <c:v>5.0635785890000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>2.305273046E-7</c:v>
+                  <c:v>4.7360860229999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>2.347261349E-7</c:v>
+                  <c:v>4.3205692569999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>2.3045494989999999E-7</c:v>
+                  <c:v>3.9786667470000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>3.074821937E-7</c:v>
+                  <c:v>3.865239457E-5</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>2.3043904E-7</c:v>
+                  <c:v>4.1977195429999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>2.4601350200000002E-7</c:v>
+                  <c:v>5.577806606E-5</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>2.3047708719999999E-7</c:v>
+                  <c:v>1.0998034610000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>2.326962868E-7</c:v>
+                  <c:v>6.947933288E-4</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>2.3059706429999999E-7</c:v>
+                  <c:v>9.2128142779999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>2.311335627E-7</c:v>
+                  <c:v>9.3888100980000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>2.3090580889999999E-7</c:v>
+                  <c:v>4.3416544190000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>2.306776359E-7</c:v>
+                  <c:v>4.0955429520000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>2.3189066590000001E-7</c:v>
+                  <c:v>9.2864012010000007E-5</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>2.3050258269999999E-7</c:v>
+                  <c:v>5.9285025579999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>2.3856224449999998E-7</c:v>
+                  <c:v>9.3057257139999994E-5</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>2.3044161690000001E-7</c:v>
+                  <c:v>3.9028510250000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>3.8585442329999999E-7</c:v>
+                  <c:v>6.6986719140000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>2.3045550620000001E-7</c:v>
+                  <c:v>0.4284966851</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2895,7 +2895,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5816,7 +5815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
@@ -5833,17 +5832,17 @@
         <v>1.4</v>
       </c>
       <c r="B1">
-        <v>0.99999976950000002</v>
+        <v>0.99995939199999995</v>
       </c>
       <c r="C1" s="1">
-        <v>2.3053978730000001E-7</v>
+        <v>4.0608006929999998E-5</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2">
         <f>MAX(B1:B201)</f>
-        <v>0.99999976960000003</v>
+        <v>0.99996138950000002</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5851,17 +5850,17 @@
         <v>1.401</v>
       </c>
       <c r="B2">
-        <v>0.99999976899999998</v>
+        <v>0.99993383520000001</v>
       </c>
       <c r="C2" s="1">
-        <v>2.30963743E-7</v>
+        <v>6.6164787730000002E-5</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2">
         <f>MIN(B1:B201)</f>
-        <v>0.34018122779999999</v>
+        <v>0.57150331489999995</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5869,17 +5868,17 @@
         <v>1.4019999999999999</v>
       </c>
       <c r="B3">
-        <v>0.99999976840000004</v>
+        <v>0.77410293770000005</v>
       </c>
       <c r="C3" s="1">
-        <v>2.316451382E-7</v>
+        <v>0.22589706230000001</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="2">
         <f>MAX(C1:C201)</f>
-        <v>0.65981877219999996</v>
+        <v>0.4284966851</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5887,17 +5886,17 @@
         <v>1.403</v>
       </c>
       <c r="B4">
-        <v>0.99999976950000002</v>
+        <v>0.99992241299999995</v>
       </c>
       <c r="C4" s="1">
-        <v>2.3046828349999999E-7</v>
+        <v>7.7586964230000002E-5</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="2">
         <f>MIN(C1:C204)</f>
-        <v>2.3043818249999999E-7</v>
+        <v>3.8610503850000003E-5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5905,10 +5904,10 @@
         <v>1.4039999999999999</v>
       </c>
       <c r="B5">
-        <v>0.99999916209999995</v>
+        <v>0.99996121770000002</v>
       </c>
       <c r="C5" s="1">
-        <v>8.3788037630000003E-7</v>
+        <v>3.8782293189999997E-5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -5916,10 +5915,10 @@
         <v>1.405</v>
       </c>
       <c r="B6">
-        <v>0.99999976950000002</v>
+        <v>0.99994441359999997</v>
       </c>
       <c r="C6" s="1">
-        <v>2.3048234520000001E-7</v>
+        <v>5.5586431730000003E-5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -5927,10 +5926,10 @@
         <v>1.4059999999999999</v>
       </c>
       <c r="B7">
-        <v>0.99999976859999995</v>
+        <v>0.99974407379999997</v>
       </c>
       <c r="C7" s="1">
-        <v>2.3143516839999999E-7</v>
+        <v>2.5592619869999999E-4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -5938,10 +5937,10 @@
         <v>1.407</v>
       </c>
       <c r="B8">
-        <v>0.99999976899999998</v>
+        <v>0.99736309430000003</v>
       </c>
       <c r="C8" s="1">
-        <v>2.3103116439999999E-7</v>
+        <v>2.6369057179999999E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -5949,10 +5948,10 @@
         <v>1.4079999999999999</v>
       </c>
       <c r="B9">
-        <v>0.99999976950000002</v>
+        <v>0.99986849560000002</v>
       </c>
       <c r="C9" s="1">
-        <v>2.3053394060000001E-7</v>
+        <v>1.3150441149999999E-4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -5960,10 +5959,10 @@
         <v>1.409</v>
       </c>
       <c r="B10">
-        <v>0.99999975419999998</v>
+        <v>0.99994212100000002</v>
       </c>
       <c r="C10" s="1">
-        <v>2.4581589839999999E-7</v>
+        <v>5.7879000499999997E-5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -5971,10 +5970,10 @@
         <v>1.41</v>
       </c>
       <c r="B11">
-        <v>0.99999976960000003</v>
+        <v>0.99995769850000005</v>
       </c>
       <c r="C11" s="1">
-        <v>2.3044260410000001E-7</v>
+        <v>4.2301520619999999E-5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -5982,10 +5981,10 @@
         <v>1.411</v>
       </c>
       <c r="B12">
-        <v>0.99999976660000001</v>
+        <v>0.9999612859</v>
       </c>
       <c r="C12" s="1">
-        <v>2.3343634699999999E-7</v>
+        <v>3.871409744E-5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -5993,10 +5992,10 @@
         <v>1.4119999999999999</v>
       </c>
       <c r="B13">
-        <v>0.99999976930000001</v>
+        <v>0.99996074489999998</v>
       </c>
       <c r="C13" s="1">
-        <v>2.306685992E-7</v>
+        <v>3.9255064039999997E-5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6004,10 +6003,10 @@
         <v>1.413</v>
       </c>
       <c r="B14">
-        <v>0.99999976930000001</v>
+        <v>0.9999590236</v>
       </c>
       <c r="C14" s="1">
-        <v>2.3072904550000001E-7</v>
+        <v>4.0976381100000003E-5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -6015,10 +6014,10 @@
         <v>1.4139999999999999</v>
       </c>
       <c r="B15">
-        <v>0.99999976739999996</v>
+        <v>0.9999579475</v>
       </c>
       <c r="C15" s="1">
-        <v>2.3255943160000001E-7</v>
+        <v>4.2052474260000002E-5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -6026,10 +6025,10 @@
         <v>1.415</v>
       </c>
       <c r="B16">
-        <v>0.99999976950000002</v>
+        <v>0.9999584064</v>
       </c>
       <c r="C16" s="1">
-        <v>2.304514027E-7</v>
+        <v>4.1593563580000003E-5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -6037,10 +6036,10 @@
         <v>1.4159999999999999</v>
       </c>
       <c r="B17">
-        <v>0.99999970120000004</v>
+        <v>0.99996002679999996</v>
       </c>
       <c r="C17" s="1">
-        <v>2.988315564E-7</v>
+        <v>3.9973183370000003E-5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6048,10 +6047,10 @@
         <v>1.417</v>
       </c>
       <c r="B18">
-        <v>0.99999976950000002</v>
+        <v>0.99996134579999996</v>
       </c>
       <c r="C18" s="1">
-        <v>2.3048932099999999E-7</v>
+        <v>3.8654200430000003E-5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6059,10 +6058,10 @@
         <v>1.4179999999999999</v>
       </c>
       <c r="B19">
-        <v>0.99999976850000005</v>
+        <v>0.99996006370000001</v>
       </c>
       <c r="C19" s="1">
-        <v>2.314768143E-7</v>
+        <v>3.9936312229999998E-5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6070,10 +6069,10 @@
         <v>1.419</v>
       </c>
       <c r="B20">
-        <v>0.99999976909999999</v>
+        <v>0.99995157499999998</v>
       </c>
       <c r="C20" s="1">
-        <v>2.3094197890000001E-7</v>
+        <v>4.8425036780000003E-5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -6081,10 +6080,10 @@
         <v>1.42</v>
       </c>
       <c r="B21">
-        <v>0.99999976940000002</v>
+        <v>0.9999175683</v>
       </c>
       <c r="C21" s="1">
-        <v>2.3057452610000001E-7</v>
+        <v>8.2431701340000002E-5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6092,10 +6091,10 @@
         <v>1.421</v>
       </c>
       <c r="B22">
-        <v>0.9999997638</v>
+        <v>0.99964708719999995</v>
       </c>
       <c r="C22" s="1">
-        <v>2.361711794E-7</v>
+        <v>3.5291283470000002E-4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -6103,10 +6102,10 @@
         <v>1.4219999999999999</v>
       </c>
       <c r="B23">
-        <v>0.99999976960000003</v>
+        <v>0.99818933210000005</v>
       </c>
       <c r="C23" s="1">
-        <v>2.3043865120000001E-7</v>
+        <v>1.8106678860000001E-3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6114,10 +6113,10 @@
         <v>1.423</v>
       </c>
       <c r="B24">
-        <v>0.99999975900000004</v>
+        <v>0.99990579670000002</v>
       </c>
       <c r="C24" s="1">
-        <v>2.410032331E-7</v>
+        <v>9.4203291190000002E-5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -6125,10 +6124,10 @@
         <v>1.4239999999999999</v>
       </c>
       <c r="B25">
-        <v>0.99999976950000002</v>
+        <v>0.99995857070000005</v>
       </c>
       <c r="C25" s="1">
-        <v>2.305315087E-7</v>
+        <v>4.1429328869999998E-5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -6136,10 +6135,10 @@
         <v>1.425</v>
       </c>
       <c r="B26">
-        <v>0.99999976879999997</v>
+        <v>0.99995400759999997</v>
       </c>
       <c r="C26" s="1">
-        <v>2.311614609E-7</v>
+        <v>4.5992363829999998E-5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -6147,10 +6146,10 @@
         <v>1.4259999999999999</v>
       </c>
       <c r="B27">
-        <v>0.99999976889999997</v>
+        <v>0.99976291019999997</v>
       </c>
       <c r="C27" s="1">
-        <v>2.3110017669999999E-7</v>
+        <v>2.370898474E-4</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -6158,10 +6157,10 @@
         <v>1.427</v>
       </c>
       <c r="B28">
-        <v>0.99999976950000002</v>
+        <v>0.99973956959999999</v>
       </c>
       <c r="C28" s="1">
-        <v>2.3054519800000001E-7</v>
+        <v>2.6043040009999998E-4</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -6169,10 +6168,10 @@
         <v>1.4279999999999999</v>
       </c>
       <c r="B29">
-        <v>0.99999976209999997</v>
+        <v>0.99995762479999994</v>
       </c>
       <c r="C29" s="1">
-        <v>2.3790932170000001E-7</v>
+        <v>4.2375247829999998E-5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -6180,10 +6179,10 @@
         <v>1.429</v>
       </c>
       <c r="B30">
-        <v>0.99999976960000003</v>
+        <v>0.99994062409999995</v>
       </c>
       <c r="C30" s="1">
-        <v>2.3043832259999999E-7</v>
+        <v>5.9375938280000001E-5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -6191,10 +6190,10 @@
         <v>1.43</v>
       </c>
       <c r="B31">
-        <v>0.99999975860000001</v>
+        <v>0.99132990649999997</v>
       </c>
       <c r="C31" s="1">
-        <v>2.4135524049999998E-7</v>
+        <v>8.6700935429999994E-3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -6202,10 +6201,10 @@
         <v>1.431</v>
       </c>
       <c r="B32">
-        <v>0.99999976950000002</v>
+        <v>0.99995297490000001</v>
       </c>
       <c r="C32" s="1">
-        <v>2.30521684E-7</v>
+        <v>4.7025090339999998E-5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6213,10 +6212,10 @@
         <v>1.4319999999999999</v>
       </c>
       <c r="B33">
-        <v>0.99999976869999996</v>
+        <v>0.99993490340000002</v>
       </c>
       <c r="C33" s="1">
-        <v>2.3128686930000001E-7</v>
+        <v>6.5096647460000003E-5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6224,10 +6223,10 @@
         <v>1.4330000000000001</v>
       </c>
       <c r="B34">
-        <v>0.99999976899999998</v>
+        <v>0.99960724459999994</v>
       </c>
       <c r="C34" s="1">
-        <v>2.3096623660000001E-7</v>
+        <v>3.9275537929999999E-4</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6235,10 +6234,10 @@
         <v>1.4339999999999999</v>
       </c>
       <c r="B35">
-        <v>0.99999976940000002</v>
+        <v>0.99996138950000002</v>
       </c>
       <c r="C35" s="1">
-        <v>2.3059022850000001E-7</v>
+        <v>3.8610503850000003E-5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -6246,10 +6245,10 @@
         <v>1.4350000000000001</v>
       </c>
       <c r="B36">
-        <v>0.99999976580000005</v>
+        <v>0.99932605240000005</v>
       </c>
       <c r="C36" s="1">
-        <v>2.342124193E-7</v>
+        <v>6.7394757440000005E-4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6257,10 +6256,10 @@
         <v>1.4359999999999999</v>
       </c>
       <c r="B37">
-        <v>0.99999976960000003</v>
+        <v>0.99995355500000005</v>
       </c>
       <c r="C37" s="1">
-        <v>2.3044530080000001E-7</v>
+        <v>4.6445001069999998E-5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -6268,10 +6267,10 @@
         <v>1.4370000000000001</v>
       </c>
       <c r="B38">
-        <v>0.99999968569999997</v>
+        <v>0.99985670550000005</v>
       </c>
       <c r="C38" s="1">
-        <v>3.1432991170000002E-7</v>
+        <v>1.4329449630000001E-4</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -6279,10 +6278,10 @@
         <v>1.4379999999999999</v>
       </c>
       <c r="B39">
-        <v>0.99999976950000002</v>
+        <v>0.99994336949999996</v>
       </c>
       <c r="C39" s="1">
-        <v>2.304713973E-7</v>
+        <v>5.6630522490000001E-5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -6290,10 +6289,10 @@
         <v>1.4390000000000001</v>
       </c>
       <c r="B40">
-        <v>0.99999976779999999</v>
+        <v>0.99987720889999998</v>
       </c>
       <c r="C40" s="1">
-        <v>2.321979995E-7</v>
+        <v>1.227910508E-4</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -6301,10 +6300,10 @@
         <v>1.44</v>
       </c>
       <c r="B41">
-        <v>0.99999976930000001</v>
+        <v>0.99994859970000005</v>
       </c>
       <c r="C41" s="1">
-        <v>2.306961597E-7</v>
+        <v>5.1400267119999997E-5</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6312,10 +6311,10 @@
         <v>1.4410000000000001</v>
       </c>
       <c r="B42">
-        <v>0.9999997692</v>
+        <v>0.99973471020000004</v>
       </c>
       <c r="C42" s="1">
-        <v>2.3078498720000001E-7</v>
+        <v>2.6528976839999997E-4</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -6323,10 +6322,10 @@
         <v>1.4419999999999999</v>
       </c>
       <c r="B43">
-        <v>0.99999976830000004</v>
+        <v>0.99995991139999996</v>
       </c>
       <c r="C43" s="1">
-        <v>2.3165595759999999E-7</v>
+        <v>4.0088576590000002E-5</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -6334,10 +6333,10 @@
         <v>1.4430000000000001</v>
       </c>
       <c r="B44">
-        <v>0.99999976950000002</v>
+        <v>0.99117504190000005</v>
       </c>
       <c r="C44" s="1">
-        <v>2.304987392E-7</v>
+        <v>8.8249581389999998E-3</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -6345,10 +6344,10 @@
         <v>1.444</v>
       </c>
       <c r="B45">
-        <v>0.99999975539999997</v>
+        <v>0.9999550076</v>
       </c>
       <c r="C45" s="1">
-        <v>2.446112259E-7</v>
+        <v>4.499235362E-5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -6356,10 +6355,10 @@
         <v>1.4450000000000001</v>
       </c>
       <c r="B46">
-        <v>0.99999976960000003</v>
+        <v>0.9999208758</v>
       </c>
       <c r="C46" s="1">
-        <v>2.3043818249999999E-7</v>
+        <v>7.9124231799999995E-5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -6367,10 +6366,10 @@
         <v>1.446</v>
       </c>
       <c r="B47">
-        <v>0.99999975669999996</v>
+        <v>0.99967705569999998</v>
       </c>
       <c r="C47" s="1">
-        <v>2.433029305E-7</v>
+        <v>3.229442893E-4</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6378,10 +6377,10 @@
         <v>1.4470000000000001</v>
       </c>
       <c r="B48">
-        <v>0.99999976950000002</v>
+        <v>0.99996042439999999</v>
       </c>
       <c r="C48" s="1">
-        <v>2.304991805E-7</v>
+        <v>3.9575577929999999E-5</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -6389,10 +6388,10 @@
         <v>1.448</v>
       </c>
       <c r="B49">
-        <v>0.99999976830000004</v>
+        <v>0.99991328430000004</v>
       </c>
       <c r="C49" s="1">
-        <v>2.317181291E-7</v>
+        <v>8.6715669049999998E-5</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -6400,10 +6399,10 @@
         <v>1.4490000000000001</v>
       </c>
       <c r="B50">
-        <v>0.99999976930000001</v>
+        <v>0.999102763</v>
       </c>
       <c r="C50" s="1">
-        <v>2.307480407E-7</v>
+        <v>8.9723696549999998E-4</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -6411,10 +6410,10 @@
         <v>1.45</v>
       </c>
       <c r="B51">
-        <v>0.9999997692</v>
+        <v>0.99995060499999999</v>
       </c>
       <c r="C51" s="1">
-        <v>2.3075430590000001E-7</v>
+        <v>4.9394998649999997E-5</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -6422,10 +6421,10 @@
         <v>1.4510000000000001</v>
       </c>
       <c r="B52">
-        <v>0.99999976830000004</v>
+        <v>0.99995700970000001</v>
       </c>
       <c r="C52" s="1">
-        <v>2.316625287E-7</v>
+        <v>4.2990252659999998E-5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -6433,10 +6432,10 @@
         <v>1.452</v>
       </c>
       <c r="B53">
-        <v>0.99999976950000002</v>
+        <v>0.99982867379999996</v>
       </c>
       <c r="C53" s="1">
-        <v>2.3050664829999999E-7</v>
+        <v>1.7132619090000001E-4</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -6444,10 +6443,10 @@
         <v>1.4530000000000001</v>
       </c>
       <c r="B54">
-        <v>0.99999976049999995</v>
+        <v>0.99899775499999999</v>
       </c>
       <c r="C54" s="1">
-        <v>2.3952032499999998E-7</v>
+        <v>1.002244969E-3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -6455,10 +6454,10 @@
         <v>1.454</v>
       </c>
       <c r="B55">
-        <v>0.99999976960000003</v>
+        <v>0.99992869419999997</v>
       </c>
       <c r="C55" s="1">
-        <v>2.3043966410000001E-7</v>
+        <v>7.1305785420000003E-5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -6466,10 +6465,10 @@
         <v>1.4550000000000001</v>
       </c>
       <c r="B56">
-        <v>0.99999972339999998</v>
+        <v>0.99996014720000004</v>
       </c>
       <c r="C56" s="1">
-        <v>2.7655972950000001E-7</v>
+        <v>3.9852756430000001E-5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -6477,10 +6476,10 @@
         <v>1.456</v>
       </c>
       <c r="B57">
-        <v>0.99999976950000002</v>
+        <v>0.99995694830000004</v>
       </c>
       <c r="C57" s="1">
-        <v>2.3046680750000001E-7</v>
+        <v>4.3051694829999999E-5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -6488,10 +6487,10 @@
         <v>1.4570000000000001</v>
       </c>
       <c r="B58">
-        <v>0.99999976710000005</v>
+        <v>0.9999248758</v>
       </c>
       <c r="C58" s="1">
-        <v>2.3287505670000001E-7</v>
+        <v>7.5124235449999999E-5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -6499,10 +6498,10 @@
         <v>1.458</v>
       </c>
       <c r="B59">
-        <v>0.99999976940000002</v>
+        <v>0.99976240149999995</v>
       </c>
       <c r="C59" s="1">
-        <v>2.3060247460000001E-7</v>
+        <v>2.3759845809999999E-4</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -6510,10 +6509,10 @@
         <v>1.4590000000000001</v>
       </c>
       <c r="B60">
-        <v>0.99999976889999997</v>
+        <v>0.99534515270000001</v>
       </c>
       <c r="C60" s="1">
-        <v>2.3106718260000001E-7</v>
+        <v>4.6548472999999998E-3</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -6521,10 +6520,10 @@
         <v>1.46</v>
       </c>
       <c r="B61">
-        <v>0.99999976899999998</v>
+        <v>0.99869562150000002</v>
       </c>
       <c r="C61" s="1">
-        <v>2.309817621E-7</v>
+        <v>1.3043784869999999E-3</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -6532,10 +6531,10 @@
         <v>1.4610000000000001</v>
       </c>
       <c r="B62">
-        <v>0.99999976940000002</v>
+        <v>0.99971262390000004</v>
       </c>
       <c r="C62" s="1">
-        <v>2.3063482260000001E-7</v>
+        <v>2.8737612249999999E-4</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -6543,10 +6542,10 @@
         <v>1.462</v>
       </c>
       <c r="B63">
-        <v>0.99999976769999999</v>
+        <v>0.99984201130000006</v>
       </c>
       <c r="C63" s="1">
-        <v>2.323039863E-7</v>
+        <v>1.579886857E-4</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -6554,10 +6553,10 @@
         <v>1.4630000000000001</v>
       </c>
       <c r="B64">
-        <v>0.99999976950000002</v>
+        <v>0.99987834060000003</v>
       </c>
       <c r="C64" s="1">
-        <v>2.3048456370000001E-7</v>
+        <v>1.216594168E-4</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -6565,10 +6564,10 @@
         <v>1.464</v>
       </c>
       <c r="B65">
-        <v>0.99999975640000005</v>
+        <v>0.99988547520000004</v>
       </c>
       <c r="C65" s="1">
-        <v>2.4363247789999999E-7</v>
+        <v>1.1452476710000001E-4</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -6576,10 +6575,10 @@
         <v>1.4650000000000001</v>
       </c>
       <c r="B66">
-        <v>0.99999976960000003</v>
+        <v>0.99987161560000004</v>
       </c>
       <c r="C66" s="1">
-        <v>2.3043919120000001E-7</v>
+        <v>1.28384413E-4</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6587,10 +6586,10 @@
         <v>1.466</v>
       </c>
       <c r="B67">
-        <v>0.99999970380000003</v>
+        <v>0.99981986720000005</v>
       </c>
       <c r="C67" s="1">
-        <v>2.9622215670000002E-7</v>
+        <v>1.8013280010000001E-4</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -6598,10 +6597,10 @@
         <v>1.4670000000000001</v>
       </c>
       <c r="B68">
-        <v>0.99999976950000002</v>
+        <v>0.99961508239999997</v>
       </c>
       <c r="C68" s="1">
-        <v>2.304578414E-7</v>
+        <v>3.8491758929999999E-4</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -6609,10 +6608,10 @@
         <v>1.468</v>
       </c>
       <c r="B69">
-        <v>0.99999976589999995</v>
+        <v>0.99638030180000003</v>
       </c>
       <c r="C69" s="1">
-        <v>2.3408075370000001E-7</v>
+        <v>3.6196981719999999E-3</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6620,10 +6619,10 @@
         <v>1.4690000000000001</v>
       </c>
       <c r="B70">
-        <v>0.99999976950000002</v>
+        <v>0.99874250369999995</v>
       </c>
       <c r="C70" s="1">
-        <v>2.3054389349999999E-7</v>
+        <v>1.257496343E-3</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -6631,10 +6630,10 @@
         <v>1.47</v>
       </c>
       <c r="B71">
-        <v>0.99999976850000005</v>
+        <v>0.99984043690000002</v>
       </c>
       <c r="C71" s="1">
-        <v>2.314723027E-7</v>
+        <v>1.5956313800000001E-4</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -6642,10 +6641,10 @@
         <v>1.4710000000000001</v>
       </c>
       <c r="B72">
-        <v>0.99999976930000001</v>
+        <v>0.99993818229999998</v>
       </c>
       <c r="C72" s="1">
-        <v>2.3074298290000001E-7</v>
+        <v>6.1817680940000005E-5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -6653,10 +6652,10 @@
         <v>1.472</v>
       </c>
       <c r="B73">
-        <v>0.9999997692</v>
+        <v>0.99995973400000004</v>
       </c>
       <c r="C73" s="1">
-        <v>2.3083365650000001E-7</v>
+        <v>4.0265960210000001E-5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6664,10 +6663,10 @@
         <v>1.4730000000000001</v>
       </c>
       <c r="B74">
-        <v>0.99999976879999997</v>
+        <v>0.99995744480000004</v>
       </c>
       <c r="C74" s="1">
-        <v>2.3120832490000001E-7</v>
+        <v>4.2555186469999999E-5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -6675,10 +6674,10 @@
         <v>1.474</v>
       </c>
       <c r="B75">
-        <v>0.99999976940000002</v>
+        <v>0.99990420369999999</v>
       </c>
       <c r="C75" s="1">
-        <v>2.3059204749999999E-7</v>
+        <v>9.5796267729999997E-5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -6686,10 +6685,10 @@
         <v>1.4750000000000001</v>
       </c>
       <c r="B76">
-        <v>0.99999976739999996</v>
+        <v>0.98686493220000004</v>
       </c>
       <c r="C76" s="1">
-        <v>2.325662322E-7</v>
+        <v>1.313506777E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -6697,10 +6696,10 @@
         <v>1.476</v>
       </c>
       <c r="B77">
-        <v>0.99999976950000002</v>
+        <v>0.99989175109999995</v>
       </c>
       <c r="C77" s="1">
-        <v>2.3048605309999999E-7</v>
+        <v>1.0824894640000001E-4</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -6708,10 +6707,10 @@
         <v>1.4770000000000001</v>
       </c>
       <c r="B78">
-        <v>0.99999976040000005</v>
+        <v>0.99996009350000004</v>
       </c>
       <c r="C78" s="1">
-        <v>2.396416645E-7</v>
+        <v>3.9906541720000001E-5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -6719,10 +6718,10 @@
         <v>1.478</v>
       </c>
       <c r="B79">
-        <v>0.99999976960000003</v>
+        <v>0.99994124350000002</v>
       </c>
       <c r="C79" s="1">
-        <v>2.3044377779999999E-7</v>
+        <v>5.8756486689999999E-5</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -6730,10 +6729,10 @@
         <v>1.4790000000000001</v>
       </c>
       <c r="B80">
-        <v>0.99999707230000001</v>
+        <v>0.99352246980000003</v>
       </c>
       <c r="C80" s="1">
-        <v>2.9277270639999999E-6</v>
+        <v>6.4775301570000002E-3</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -6741,10 +6740,10 @@
         <v>1.48</v>
       </c>
       <c r="B81">
-        <v>0.99999976960000003</v>
+        <v>0.99993166779999998</v>
       </c>
       <c r="C81" s="1">
-        <v>2.3044134370000001E-7</v>
+        <v>6.8332177250000006E-5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -6752,10 +6751,10 @@
         <v>1.4810000000000001</v>
       </c>
       <c r="B82">
-        <v>0.99999975640000005</v>
+        <v>0.99995863200000001</v>
       </c>
       <c r="C82" s="1">
-        <v>2.4362467690000001E-7</v>
+        <v>4.1367956700000002E-5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -6763,10 +6762,10 @@
         <v>1.482</v>
       </c>
       <c r="B83">
-        <v>0.99999976950000002</v>
+        <v>0.99944949370000002</v>
       </c>
       <c r="C83" s="1">
-        <v>2.3047264120000001E-7</v>
+        <v>5.5050625099999995E-4</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -6774,10 +6773,10 @@
         <v>1.4830000000000001</v>
       </c>
       <c r="B84">
-        <v>0.9999997665</v>
+        <v>0.99992962110000005</v>
       </c>
       <c r="C84" s="1">
-        <v>2.334504275E-7</v>
+        <v>7.0378924260000006E-5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -6785,10 +6784,10 @@
         <v>1.484</v>
       </c>
       <c r="B85">
-        <v>0.99999976950000002</v>
+        <v>0.99995377259999996</v>
       </c>
       <c r="C85" s="1">
-        <v>2.305420049E-7</v>
+        <v>4.6227376790000001E-5</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -6796,10 +6795,10 @@
         <v>1.4850000000000001</v>
       </c>
       <c r="B86">
-        <v>0.99999976830000004</v>
+        <v>0.99066593830000005</v>
       </c>
       <c r="C86" s="1">
-        <v>2.3166058569999999E-7</v>
+        <v>9.3340617389999995E-3</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -6807,10 +6806,10 @@
         <v>1.486</v>
       </c>
       <c r="B87">
-        <v>0.99999976930000001</v>
+        <v>0.99995919779999998</v>
       </c>
       <c r="C87" s="1">
-        <v>2.3066497619999999E-7</v>
+        <v>4.080221217E-5</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -6818,10 +6817,10 @@
         <v>1.4870000000000001</v>
       </c>
       <c r="B88">
-        <v>0.99999976899999998</v>
+        <v>0.99981659590000005</v>
       </c>
       <c r="C88" s="1">
-        <v>2.3104181430000001E-7</v>
+        <v>1.8340414600000001E-4</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -6829,10 +6828,10 @@
         <v>1.488</v>
       </c>
       <c r="B89">
-        <v>0.99999976909999999</v>
+        <v>0.99993839920000005</v>
       </c>
       <c r="C89" s="1">
-        <v>2.3087633899999999E-7</v>
+        <v>6.1600821439999998E-5</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -6840,10 +6839,10 @@
         <v>1.4890000000000001</v>
       </c>
       <c r="B90">
-        <v>0.9999997692</v>
+        <v>0.99992293809999999</v>
       </c>
       <c r="C90" s="1">
-        <v>2.307590936E-7</v>
+        <v>7.7061856030000004E-5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -6851,10 +6850,10 @@
         <v>1.49</v>
       </c>
       <c r="B91">
-        <v>0.99999976869999996</v>
+        <v>0.99991087670000001</v>
       </c>
       <c r="C91" s="1">
-        <v>2.312536772E-7</v>
+        <v>8.9123311180000001E-5</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -6862,10 +6861,10 @@
         <v>1.4910000000000001</v>
       </c>
       <c r="B92">
-        <v>0.99999976940000002</v>
+        <v>0.99993363189999995</v>
       </c>
       <c r="C92" s="1">
-        <v>2.306099544E-7</v>
+        <v>6.6368127200000003E-5</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -6873,10 +6872,10 @@
         <v>1.492</v>
       </c>
       <c r="B93">
-        <v>0.99999976800000001</v>
+        <v>0.99991710739999995</v>
       </c>
       <c r="C93" s="1">
-        <v>2.3198943339999999E-7</v>
+        <v>8.2892625919999999E-5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -6884,10 +6883,10 @@
         <v>1.4930000000000001</v>
       </c>
       <c r="B94">
-        <v>0.99999976950000002</v>
+        <v>0.99991143790000003</v>
       </c>
       <c r="C94" s="1">
-        <v>2.305254543E-7</v>
+        <v>8.8562148310000006E-5</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -6895,10 +6894,10 @@
         <v>1.494</v>
       </c>
       <c r="B95">
-        <v>0.99999976629999998</v>
+        <v>0.99994621019999996</v>
       </c>
       <c r="C95" s="1">
-        <v>2.3366072889999999E-7</v>
+        <v>5.378976086E-5</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -6906,10 +6905,10 @@
         <v>1.4950000000000001</v>
       </c>
       <c r="B96">
-        <v>0.99999976950000002</v>
+        <v>0.99966765909999999</v>
       </c>
       <c r="C96" s="1">
-        <v>2.3047688809999999E-7</v>
+        <v>3.3234086359999998E-4</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -6917,10 +6916,10 @@
         <v>1.496</v>
       </c>
       <c r="B97">
-        <v>0.99999976130000001</v>
+        <v>0.99996117100000004</v>
       </c>
       <c r="C97" s="1">
-        <v>2.3866597280000002E-7</v>
+        <v>3.8829012670000002E-5</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -6928,10 +6927,10 @@
         <v>1.4970000000000001</v>
       </c>
       <c r="B98">
-        <v>0.99999976950000002</v>
+        <v>0.99938248399999996</v>
       </c>
       <c r="C98" s="1">
-        <v>2.304505959E-7</v>
+        <v>6.1751595630000003E-4</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -6939,10 +6938,10 @@
         <v>1.498</v>
       </c>
       <c r="B99">
-        <v>0.999999733</v>
+        <v>0.99994051989999999</v>
       </c>
       <c r="C99" s="1">
-        <v>2.6698977380000002E-7</v>
+        <v>5.94801035E-5</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -6950,10 +6949,10 @@
         <v>1.4990000000000001</v>
       </c>
       <c r="B100">
-        <v>0.99999976960000003</v>
+        <v>0.99995017320000001</v>
       </c>
       <c r="C100" s="1">
-        <v>2.304394234E-7</v>
+        <v>4.9826769390000001E-5</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -6961,10 +6960,10 @@
         <v>1.5</v>
       </c>
       <c r="B101">
-        <v>0.34018122779999999</v>
+        <v>0.57150331489999995</v>
       </c>
       <c r="C101" s="1">
-        <v>0.65981877219999996</v>
+        <v>0.4284966851</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -6972,10 +6971,10 @@
         <v>1.5009999999999999</v>
       </c>
       <c r="B102">
-        <v>0.99999976960000003</v>
+        <v>0.99994686870000005</v>
       </c>
       <c r="C102" s="1">
-        <v>2.3043932369999999E-7</v>
+        <v>5.3131317670000002E-5</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -6983,10 +6982,10 @@
         <v>1.502</v>
       </c>
       <c r="B103">
-        <v>0.99999972640000001</v>
+        <v>0.99995406050000002</v>
       </c>
       <c r="C103" s="1">
-        <v>2.7361736700000002E-7</v>
+        <v>4.593946118E-5</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -6994,10 +6993,10 @@
         <v>1.5029999999999999</v>
       </c>
       <c r="B104">
-        <v>0.99999976960000003</v>
+        <v>0.99937763820000003</v>
       </c>
       <c r="C104" s="1">
-        <v>2.3044782380000001E-7</v>
+        <v>6.2236176299999997E-4</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -7005,10 +7004,10 @@
         <v>1.504</v>
       </c>
       <c r="B105">
-        <v>0.99999975799999996</v>
+        <v>0.99987996980000005</v>
       </c>
       <c r="C105" s="1">
-        <v>2.4201199670000001E-7</v>
+        <v>1.200302451E-4</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -7016,10 +7015,10 @@
         <v>1.5049999999999999</v>
       </c>
       <c r="B106">
-        <v>0.99999976950000002</v>
+        <v>0.99996023020000002</v>
       </c>
       <c r="C106" s="1">
-        <v>2.3046325080000001E-7</v>
+        <v>3.9769848569999998E-5</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -7027,10 +7026,10 @@
         <v>1.506</v>
       </c>
       <c r="B107">
-        <v>0.99999976410000002</v>
+        <v>0.99994566080000002</v>
       </c>
       <c r="C107" s="1">
-        <v>2.359271893E-7</v>
+        <v>5.4339213339999999E-5</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -7038,10 +7037,10 @@
         <v>1.5069999999999999</v>
       </c>
       <c r="B108">
-        <v>0.99999976950000002</v>
+        <v>0.99959974200000001</v>
       </c>
       <c r="C108" s="1">
-        <v>2.304842972E-7</v>
+        <v>4.0025799429999997E-4</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -7049,10 +7048,10 @@
         <v>1.508</v>
       </c>
       <c r="B109">
-        <v>0.99999976629999998</v>
+        <v>0.99960430280000001</v>
       </c>
       <c r="C109" s="1">
-        <v>2.3372676820000001E-7</v>
+        <v>3.9569715030000001E-4</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -7060,10 +7059,10 @@
         <v>1.5089999999999999</v>
       </c>
       <c r="B110">
-        <v>0.99999976950000002</v>
+        <v>0.99993653689999995</v>
       </c>
       <c r="C110" s="1">
-        <v>2.305097523E-7</v>
+        <v>6.3463143110000005E-5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -7071,10 +7070,10 @@
         <v>1.51</v>
       </c>
       <c r="B111">
-        <v>0.99999976729999995</v>
+        <v>0.99996044139999996</v>
       </c>
       <c r="C111" s="1">
-        <v>2.3268193140000001E-7</v>
+        <v>3.9558598330000003E-5</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -7082,10 +7081,10 @@
         <v>1.5109999999999999</v>
       </c>
       <c r="B112">
-        <v>0.99999976950000002</v>
+        <v>0.9999574309</v>
       </c>
       <c r="C112" s="1">
-        <v>2.3053832749999999E-7</v>
+        <v>4.2569108459999999E-5</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -7093,10 +7092,10 @@
         <v>1.512</v>
       </c>
       <c r="B113">
-        <v>0.9999997679</v>
+        <v>0.99993150590000002</v>
       </c>
       <c r="C113" s="1">
-        <v>2.321052871E-7</v>
+        <v>6.8494124189999998E-5</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -7104,10 +7103,10 @@
         <v>1.5129999999999999</v>
       </c>
       <c r="B114">
-        <v>0.99999976940000002</v>
+        <v>0.99982656749999999</v>
       </c>
       <c r="C114" s="1">
-        <v>2.3056855099999999E-7</v>
+        <v>1.7343253359999999E-4</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -7115,10 +7114,10 @@
         <v>1.514</v>
       </c>
       <c r="B115">
-        <v>0.99999976820000003</v>
+        <v>0.99888925210000001</v>
       </c>
       <c r="C115" s="1">
-        <v>2.3175688600000001E-7</v>
+        <v>1.1107479070000001E-3</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -7126,10 +7125,10 @@
         <v>1.5149999999999999</v>
       </c>
       <c r="B116">
-        <v>0.99999976940000002</v>
+        <v>0.99029413249999998</v>
       </c>
       <c r="C116" s="1">
-        <v>2.3059872989999999E-7</v>
+        <v>9.7058675489999999E-3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -7137,10 +7136,10 @@
         <v>1.516</v>
       </c>
       <c r="B117">
-        <v>0.99999976850000005</v>
+        <v>0.99940634719999999</v>
       </c>
       <c r="C117" s="1">
-        <v>2.315349503E-7</v>
+        <v>5.9365283949999997E-4</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -7148,10 +7147,10 @@
         <v>1.5169999999999999</v>
       </c>
       <c r="B118">
-        <v>0.99999976940000002</v>
+        <v>0.99974394109999998</v>
       </c>
       <c r="C118" s="1">
-        <v>2.3062698709999999E-7</v>
+        <v>2.5605885190000001E-4</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -7159,10 +7158,10 @@
         <v>1.518</v>
       </c>
       <c r="B119">
-        <v>0.99999976859999995</v>
+        <v>0.99982276569999995</v>
       </c>
       <c r="C119" s="1">
-        <v>2.313904414E-7</v>
+        <v>1.7723428050000001E-4</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -7170,10 +7169,10 @@
         <v>1.5189999999999999</v>
       </c>
       <c r="B120">
-        <v>0.99999976930000001</v>
+        <v>0.99984274829999997</v>
       </c>
       <c r="C120" s="1">
-        <v>2.3065137640000001E-7</v>
+        <v>1.572517208E-4</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -7181,10 +7180,10 @@
         <v>1.52</v>
       </c>
       <c r="B121">
-        <v>0.99999976869999996</v>
+        <v>0.99983039819999997</v>
       </c>
       <c r="C121" s="1">
-        <v>2.312977023E-7</v>
+        <v>1.6960184250000001E-4</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -7192,10 +7191,10 @@
         <v>1.5209999999999999</v>
       </c>
       <c r="B122">
-        <v>0.99999976930000001</v>
+        <v>0.99977044449999997</v>
       </c>
       <c r="C122" s="1">
-        <v>2.3067006699999999E-7</v>
+        <v>2.2955551850000001E-4</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -7203,10 +7202,10 @@
         <v>1.522</v>
       </c>
       <c r="B123">
-        <v>0.99999976879999997</v>
+        <v>0.99954047619999997</v>
       </c>
       <c r="C123" s="1">
-        <v>2.312427682E-7</v>
+        <v>4.595237992E-4</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -7214,10 +7213,10 @@
         <v>1.5229999999999999</v>
       </c>
       <c r="B124">
-        <v>0.99999976930000001</v>
+        <v>0.99691584840000003</v>
       </c>
       <c r="C124" s="1">
-        <v>2.3068156319999999E-7</v>
+        <v>3.0841516299999999E-3</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -7225,10 +7224,10 @@
         <v>1.524</v>
       </c>
       <c r="B125">
-        <v>0.99999976879999997</v>
+        <v>0.9974927039</v>
       </c>
       <c r="C125" s="1">
-        <v>2.3121824329999999E-7</v>
+        <v>2.5072960509999998E-3</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -7236,10 +7235,10 @@
         <v>1.5249999999999999</v>
       </c>
       <c r="B126">
-        <v>0.99999976930000001</v>
+        <v>0.99976055789999996</v>
       </c>
       <c r="C126" s="1">
-        <v>2.306849152E-7</v>
+        <v>2.3944214650000001E-4</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -7247,10 +7246,10 @@
         <v>1.526</v>
       </c>
       <c r="B127">
-        <v>0.99999976879999997</v>
+        <v>0.99991779179999996</v>
       </c>
       <c r="C127" s="1">
-        <v>2.3122098910000001E-7</v>
+        <v>8.22081809E-5</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -7258,10 +7257,10 @@
         <v>1.5269999999999999</v>
       </c>
       <c r="B128">
-        <v>0.99999976930000001</v>
+        <v>0.99995362300000001</v>
       </c>
       <c r="C128" s="1">
-        <v>2.3067986379999999E-7</v>
+        <v>4.637698821E-5</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -7269,10 +7268,10 @@
         <v>1.528</v>
       </c>
       <c r="B129">
-        <v>0.99999976869999996</v>
+        <v>0.9999613678</v>
       </c>
       <c r="C129" s="1">
-        <v>2.3125122689999999E-7</v>
+        <v>3.8632215389999997E-5</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -7280,10 +7279,10 @@
         <v>1.5289999999999999</v>
       </c>
       <c r="B130">
-        <v>0.99999976930000001</v>
+        <v>0.9999485186</v>
       </c>
       <c r="C130" s="1">
-        <v>2.3066687749999999E-7</v>
+        <v>5.1481385129999998E-5</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -7291,10 +7290,10 @@
         <v>1.53</v>
       </c>
       <c r="B131">
-        <v>0.99999976869999996</v>
+        <v>0.99982834939999998</v>
       </c>
       <c r="C131" s="1">
-        <v>2.3131258199999999E-7</v>
+        <v>1.7165058499999999E-4</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -7302,10 +7301,10 @@
         <v>1.5309999999999999</v>
       </c>
       <c r="B132">
-        <v>0.99999976940000002</v>
+        <v>0.99699477079999999</v>
       </c>
       <c r="C132" s="1">
-        <v>2.306470744E-7</v>
+        <v>3.0052292049999999E-3</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -7313,10 +7312,10 @@
         <v>1.532</v>
       </c>
       <c r="B133">
-        <v>0.99999976859999995</v>
+        <v>0.99992075130000002</v>
       </c>
       <c r="C133" s="1">
-        <v>2.31413085E-7</v>
+        <v>7.9248652110000003E-5</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -7324,10 +7323,10 @@
         <v>1.5329999999999999</v>
       </c>
       <c r="B134">
-        <v>0.99999976940000002</v>
+        <v>0.99996108459999999</v>
       </c>
       <c r="C134" s="1">
-        <v>2.3062204879999999E-7</v>
+        <v>3.8915431740000002E-5</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -7335,10 +7334,10 @@
         <v>1.534</v>
       </c>
       <c r="B135">
-        <v>0.99999976840000004</v>
+        <v>0.99993692850000004</v>
       </c>
       <c r="C135" s="1">
-        <v>2.3156765470000001E-7</v>
+        <v>6.3071473739999994E-5</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -7346,10 +7345,10 @@
         <v>1.5349999999999999</v>
       </c>
       <c r="B136">
-        <v>0.99999976940000002</v>
+        <v>0.99433581999999998</v>
       </c>
       <c r="C136" s="1">
-        <v>2.3059365160000001E-7</v>
+        <v>5.6641800080000004E-3</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -7357,10 +7356,10 @@
         <v>1.536</v>
       </c>
       <c r="B137">
-        <v>0.99999976820000003</v>
+        <v>0.99992301920000004</v>
       </c>
       <c r="C137" s="1">
-        <v>2.31803548E-7</v>
+        <v>7.6980817890000001E-5</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -7368,10 +7367,10 @@
         <v>1.5369999999999999</v>
       </c>
       <c r="B138">
-        <v>0.99999976940000002</v>
+        <v>0.99996069499999996</v>
       </c>
       <c r="C138" s="1">
-        <v>2.3056377920000001E-7</v>
+        <v>3.9304988819999997E-5</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -7379,10 +7378,10 @@
         <v>1.538</v>
       </c>
       <c r="B139">
-        <v>0.99999976779999999</v>
+        <v>0.99980952609999996</v>
       </c>
       <c r="C139" s="1">
-        <v>2.3217277569999999E-7</v>
+        <v>1.904738684E-4</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -7390,10 +7389,10 @@
         <v>1.5389999999999999</v>
       </c>
       <c r="B140">
-        <v>0.99999976950000002</v>
+        <v>0.99986259430000002</v>
       </c>
       <c r="C140" s="1">
-        <v>2.305342102E-7</v>
+        <v>1.3740569449999999E-4</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -7401,10 +7400,10 @@
         <v>1.54</v>
       </c>
       <c r="B141">
-        <v>0.99999976719999994</v>
+        <v>0.99996124710000001</v>
       </c>
       <c r="C141" s="1">
-        <v>2.3278328089999999E-7</v>
+        <v>3.8752937859999999E-5</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -7412,10 +7411,10 @@
         <v>1.5409999999999999</v>
       </c>
       <c r="B142">
-        <v>0.99999976950000002</v>
+        <v>0.99972547810000001</v>
       </c>
       <c r="C142" s="1">
-        <v>2.305065134E-7</v>
+        <v>2.7452194129999998E-4</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -7423,10 +7422,10 @@
         <v>1.542</v>
       </c>
       <c r="B143">
-        <v>0.99999976609999996</v>
+        <v>0.9999244008</v>
       </c>
       <c r="C143" s="1">
-        <v>2.338897243E-7</v>
+        <v>7.5599163030000001E-5</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -7434,10 +7433,10 @@
         <v>1.5429999999999999</v>
       </c>
       <c r="B144">
-        <v>0.99999976950000002</v>
+        <v>0.99995229809999997</v>
       </c>
       <c r="C144" s="1">
-        <v>2.3048203070000001E-7</v>
+        <v>4.770191941E-5</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -7445,10 +7444,10 @@
         <v>1.544</v>
       </c>
       <c r="B145">
-        <v>0.9999997638</v>
+        <v>0.99854328469999998</v>
       </c>
       <c r="C145" s="1">
-        <v>2.3622238899999999E-7</v>
+        <v>1.4567152800000001E-3</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -7456,10 +7455,10 @@
         <v>1.5449999999999999</v>
       </c>
       <c r="B146">
-        <v>0.99999976950000002</v>
+        <v>0.99996116719999995</v>
       </c>
       <c r="C146" s="1">
-        <v>2.304619231E-7</v>
+        <v>3.8832843970000003E-5</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -7467,10 +7466,10 @@
         <v>1.546</v>
       </c>
       <c r="B147">
-        <v>0.99999975730000001</v>
+        <v>0.99943753319999995</v>
       </c>
       <c r="C147" s="1">
-        <v>2.4268385559999998E-7</v>
+        <v>5.6246680240000003E-4</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -7478,10 +7477,10 @@
         <v>1.5469999999999999</v>
       </c>
       <c r="B148">
-        <v>0.99999976960000003</v>
+        <v>0.99995449030000005</v>
       </c>
       <c r="C148" s="1">
-        <v>2.3044727499999999E-7</v>
+        <v>4.5509734060000001E-5</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -7489,10 +7488,10 @@
         <v>1.548</v>
       </c>
       <c r="B149">
-        <v>0.99999972370000001</v>
+        <v>0.99982462729999999</v>
       </c>
       <c r="C149" s="1">
-        <v>2.7632079480000001E-7</v>
+        <v>1.7537272560000001E-4</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -7500,10 +7499,10 @@
         <v>1.5489999999999999</v>
       </c>
       <c r="B150">
-        <v>0.99999976960000003</v>
+        <v>0.99994867939999998</v>
       </c>
       <c r="C150" s="1">
-        <v>2.304392532E-7</v>
+        <v>5.1320573069999999E-5</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -7511,10 +7510,10 @@
         <v>1.55</v>
       </c>
       <c r="B151">
-        <v>0.34018122779999999</v>
+        <v>0.99983686230000002</v>
       </c>
       <c r="C151" s="1">
-        <v>0.65981877219999996</v>
+        <v>1.6313768640000001E-4</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -7522,10 +7521,10 @@
         <v>1.5509999999999999</v>
       </c>
       <c r="B152">
-        <v>0.99999976960000003</v>
+        <v>0.99995286159999996</v>
       </c>
       <c r="C152" s="1">
-        <v>2.304393406E-7</v>
+        <v>4.7138380119999999E-5</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -7533,10 +7532,10 @@
         <v>1.552</v>
       </c>
       <c r="B153">
-        <v>0.9999997303</v>
+        <v>0.99962112759999999</v>
       </c>
       <c r="C153" s="1">
-        <v>2.6969389080000002E-7</v>
+        <v>3.7887237270000003E-4</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -7544,10 +7543,10 @@
         <v>1.5529999999999999</v>
       </c>
       <c r="B154">
-        <v>0.99999976960000003</v>
+        <v>0.99996043229999998</v>
       </c>
       <c r="C154" s="1">
-        <v>2.304497005E-7</v>
+        <v>3.9567738049999997E-5</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -7555,10 +7554,10 @@
         <v>1.554</v>
       </c>
       <c r="B155">
-        <v>0.99999976069999996</v>
+        <v>0.98980068929999998</v>
       </c>
       <c r="C155" s="1">
-        <v>2.393391829E-7</v>
+        <v>1.01993107E-2</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -7566,10 +7565,10 @@
         <v>1.5549999999999999</v>
       </c>
       <c r="B156">
-        <v>0.99999976950000002</v>
+        <v>0.99995693860000001</v>
       </c>
       <c r="C156" s="1">
-        <v>2.3047380159999999E-7</v>
+        <v>4.3061404710000003E-5</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -7577,10 +7576,10 @@
         <v>1.556</v>
       </c>
       <c r="B157">
-        <v>0.99999976599999996</v>
+        <v>0.99989390909999998</v>
       </c>
       <c r="C157" s="1">
-        <v>2.3395788410000001E-7</v>
+        <v>1.060908947E-4</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -7588,10 +7587,10 @@
         <v>1.5569999999999999</v>
       </c>
       <c r="B158">
-        <v>0.99999976950000002</v>
+        <v>0.99986242280000004</v>
       </c>
       <c r="C158" s="1">
-        <v>2.3051760669999999E-7</v>
+        <v>1.3757724960000001E-4</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -7599,10 +7598,10 @@
         <v>1.5580000000000001</v>
       </c>
       <c r="B159">
-        <v>0.99999976779999999</v>
+        <v>0.99996063859999995</v>
       </c>
       <c r="C159" s="1">
-        <v>2.321548503E-7</v>
+        <v>3.936141365E-5</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -7610,10 +7609,10 @@
         <v>1.5589999999999999</v>
       </c>
       <c r="B160">
-        <v>0.99999976940000002</v>
+        <v>0.99963125959999999</v>
       </c>
       <c r="C160" s="1">
-        <v>2.305920839E-7</v>
+        <v>3.687403763E-4</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -7621,10 +7620,10 @@
         <v>1.56</v>
       </c>
       <c r="B161">
-        <v>0.99999976859999995</v>
+        <v>0.99991250210000004</v>
       </c>
       <c r="C161" s="1">
-        <v>2.3135783340000001E-7</v>
+        <v>8.7497919250000006E-5</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -7632,10 +7631,10 @@
         <v>1.5609999999999999</v>
       </c>
       <c r="B162">
-        <v>0.99999976930000001</v>
+        <v>0.99996041719999995</v>
       </c>
       <c r="C162" s="1">
-        <v>2.3071913899999999E-7</v>
+        <v>3.9582835309999997E-5</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -7643,10 +7642,10 @@
         <v>1.5620000000000001</v>
       </c>
       <c r="B163">
-        <v>0.99999976909999999</v>
+        <v>0.99980398339999998</v>
       </c>
       <c r="C163" s="1">
-        <v>2.309467264E-7</v>
+        <v>1.9601663139999999E-4</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -7654,10 +7653,10 @@
         <v>1.5629999999999999</v>
       </c>
       <c r="B164">
-        <v>0.99999976909999999</v>
+        <v>0.99979377729999996</v>
       </c>
       <c r="C164" s="1">
-        <v>2.3094770370000001E-7</v>
+        <v>2.0622267300000001E-4</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -7665,10 +7664,10 @@
         <v>1.5640000000000001</v>
       </c>
       <c r="B165">
-        <v>0.99999976930000001</v>
+        <v>0.99995847090000001</v>
       </c>
       <c r="C165" s="1">
-        <v>2.30714216E-7</v>
+        <v>4.1529124099999999E-5</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -7676,10 +7675,10 @@
         <v>1.5649999999999999</v>
       </c>
       <c r="B166">
-        <v>0.99999976859999995</v>
+        <v>0.99994779050000004</v>
       </c>
       <c r="C166" s="1">
-        <v>2.314063736E-7</v>
+        <v>5.2209521510000001E-5</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -7687,10 +7686,10 @@
         <v>1.5660000000000001</v>
       </c>
       <c r="B167">
-        <v>0.99999976940000002</v>
+        <v>0.99948660180000004</v>
       </c>
       <c r="C167" s="1">
-        <v>2.30576273E-7</v>
+        <v>5.133981914E-4</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -7698,10 +7697,10 @@
         <v>1.5669999999999999</v>
       </c>
       <c r="B168">
-        <v>0.99999976749999997</v>
+        <v>0.99978001699999997</v>
       </c>
       <c r="C168" s="1">
-        <v>2.325320109E-7</v>
+        <v>2.199829933E-4</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -7709,10 +7708,10 @@
         <v>1.5680000000000001</v>
       </c>
       <c r="B169">
-        <v>0.99999976950000002</v>
+        <v>0.99995094679999996</v>
       </c>
       <c r="C169" s="1">
-        <v>2.3049462119999999E-7</v>
+        <v>4.9053235049999998E-5</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -7720,10 +7719,10 @@
         <v>1.569</v>
       </c>
       <c r="B170">
-        <v>0.99999976329999996</v>
+        <v>0.9999607439</v>
       </c>
       <c r="C170" s="1">
-        <v>2.367156594E-7</v>
+        <v>3.9256098470000002E-5</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -7731,10 +7730,10 @@
         <v>1.57</v>
       </c>
       <c r="B171">
-        <v>0.99999976950000002</v>
+        <v>0.99993521490000004</v>
       </c>
       <c r="C171" s="1">
-        <v>2.304510941E-7</v>
+        <v>6.4785090479999995E-5</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -7742,10 +7741,10 @@
         <v>1.571</v>
       </c>
       <c r="B172">
-        <v>0.99999970140000005</v>
+        <v>0.99970333050000004</v>
       </c>
       <c r="C172" s="1">
-        <v>2.986279805E-7</v>
+        <v>2.9666945419999999E-4</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -7753,10 +7752,10 @@
         <v>1.5720000000000001</v>
       </c>
       <c r="B173">
-        <v>0.99999976960000003</v>
+        <v>0.99585628079999999</v>
       </c>
       <c r="C173" s="1">
-        <v>2.3043823260000001E-7</v>
+        <v>4.1437191959999998E-3</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -7764,10 +7763,10 @@
         <v>1.573</v>
       </c>
       <c r="B174">
-        <v>0.99999973070000003</v>
+        <v>0.99983951029999996</v>
       </c>
       <c r="C174" s="1">
-        <v>2.6925280840000001E-7</v>
+        <v>1.6048974050000001E-4</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -7775,10 +7774,10 @@
         <v>1.5740000000000001</v>
       </c>
       <c r="B175">
-        <v>0.99999976950000002</v>
+        <v>0.99993497539999998</v>
       </c>
       <c r="C175" s="1">
-        <v>2.3045646970000001E-7</v>
+        <v>6.5024635949999997E-5</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -7786,10 +7785,10 @@
         <v>1.575</v>
       </c>
       <c r="B176">
-        <v>0.99999976499999998</v>
+        <v>0.99995548010000002</v>
       </c>
       <c r="C176" s="1">
-        <v>2.3504335219999999E-7</v>
+        <v>4.4519864950000002E-5</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -7797,10 +7796,10 @@
         <v>1.5760000000000001</v>
       </c>
       <c r="B177">
-        <v>0.99999976950000002</v>
+        <v>0.99996097589999999</v>
       </c>
       <c r="C177" s="1">
-        <v>2.305159188E-7</v>
+        <v>3.9024149390000002E-5</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -7808,10 +7807,10 @@
         <v>1.577</v>
       </c>
       <c r="B178">
-        <v>0.99999976810000002</v>
+        <v>0.99996084689999998</v>
       </c>
       <c r="C178" s="1">
-        <v>2.319061618E-7</v>
+        <v>3.915310307E-5</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -7819,10 +7818,10 @@
         <v>1.5780000000000001</v>
       </c>
       <c r="B179">
-        <v>0.99999976940000002</v>
+        <v>0.9999579072</v>
       </c>
       <c r="C179" s="1">
-        <v>2.306461141E-7</v>
+        <v>4.2092825300000001E-5</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -7830,10 +7829,10 @@
         <v>1.579</v>
       </c>
       <c r="B180">
-        <v>0.99999976899999998</v>
+        <v>0.99995378690000003</v>
       </c>
       <c r="C180" s="1">
-        <v>2.310353532E-7</v>
+        <v>4.62130988E-5</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -7841,10 +7840,10 @@
         <v>1.58</v>
       </c>
       <c r="B181">
-        <v>0.99999976909999999</v>
+        <v>0.99995009619999997</v>
       </c>
       <c r="C181" s="1">
-        <v>2.309318941E-7</v>
+        <v>4.9903782309999997E-5</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -7852,10 +7851,10 @@
         <v>1.581</v>
       </c>
       <c r="B182">
-        <v>0.99999976930000001</v>
+        <v>0.99994836330000003</v>
       </c>
       <c r="C182" s="1">
-        <v>2.306880463E-7</v>
+        <v>5.1636682540000001E-5</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -7863,10 +7862,10 @@
         <v>1.5820000000000001</v>
       </c>
       <c r="B183">
-        <v>0.99999976830000004</v>
+        <v>0.99994936420000002</v>
       </c>
       <c r="C183" s="1">
-        <v>2.316790041E-7</v>
+        <v>5.0635785890000001E-5</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -7874,10 +7873,10 @@
         <v>1.583</v>
       </c>
       <c r="B184">
-        <v>0.99999976950000002</v>
+        <v>0.99995263909999998</v>
       </c>
       <c r="C184" s="1">
-        <v>2.305273046E-7</v>
+        <v>4.7360860229999999E-5</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -7885,10 +7884,10 @@
         <v>1.5840000000000001</v>
       </c>
       <c r="B185">
-        <v>0.99999976530000001</v>
+        <v>0.99995679429999995</v>
       </c>
       <c r="C185" s="1">
-        <v>2.347261349E-7</v>
+        <v>4.3205692569999997E-5</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -7896,10 +7895,10 @@
         <v>1.585</v>
       </c>
       <c r="B186">
-        <v>0.99999976950000002</v>
+        <v>0.99996021329999996</v>
       </c>
       <c r="C186" s="1">
-        <v>2.3045494989999999E-7</v>
+        <v>3.9786667470000001E-5</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -7907,10 +7906,10 @@
         <v>1.5860000000000001</v>
       </c>
       <c r="B187">
-        <v>0.99999969249999998</v>
+        <v>0.99996134759999999</v>
       </c>
       <c r="C187" s="1">
-        <v>3.074821937E-7</v>
+        <v>3.865239457E-5</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -7918,10 +7917,10 @@
         <v>1.587</v>
       </c>
       <c r="B188">
-        <v>0.99999976960000003</v>
+        <v>0.99995802280000001</v>
       </c>
       <c r="C188" s="1">
-        <v>2.3043904E-7</v>
+        <v>4.1977195429999997E-5</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -7929,10 +7928,10 @@
         <v>1.5880000000000001</v>
       </c>
       <c r="B189">
-        <v>0.99999975399999996</v>
+        <v>0.99994422189999999</v>
       </c>
       <c r="C189" s="1">
-        <v>2.4601350200000002E-7</v>
+        <v>5.577806606E-5</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -7940,10 +7939,10 @@
         <v>1.589</v>
       </c>
       <c r="B190">
-        <v>0.99999976950000002</v>
+        <v>0.99989001970000002</v>
       </c>
       <c r="C190" s="1">
-        <v>2.3047708719999999E-7</v>
+        <v>1.0998034610000001E-4</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -7951,10 +7950,10 @@
         <v>1.59</v>
       </c>
       <c r="B191">
-        <v>0.99999976729999995</v>
+        <v>0.9993052067</v>
       </c>
       <c r="C191" s="1">
-        <v>2.326962868E-7</v>
+        <v>6.947933288E-4</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -7962,10 +7961,10 @@
         <v>1.591</v>
       </c>
       <c r="B192">
-        <v>0.99999976940000002</v>
+        <v>0.99907871859999997</v>
       </c>
       <c r="C192" s="1">
-        <v>2.3059706429999999E-7</v>
+        <v>9.2128142779999999E-4</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -7973,10 +7972,10 @@
         <v>1.5920000000000001</v>
       </c>
       <c r="B193">
-        <v>0.99999976889999997</v>
+        <v>0.99990611190000001</v>
       </c>
       <c r="C193" s="1">
-        <v>2.311335627E-7</v>
+        <v>9.3888100980000003E-5</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -7984,10 +7983,10 @@
         <v>1.593</v>
       </c>
       <c r="B194">
-        <v>0.99999976909999999</v>
+        <v>0.99995658350000005</v>
       </c>
       <c r="C194" s="1">
-        <v>2.3090580889999999E-7</v>
+        <v>4.3416544190000001E-5</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -7995,10 +7994,10 @@
         <v>1.5940000000000001</v>
       </c>
       <c r="B195">
-        <v>0.99999976930000001</v>
+        <v>0.99995904459999996</v>
       </c>
       <c r="C195" s="1">
-        <v>2.306776359E-7</v>
+        <v>4.0955429520000001E-5</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -8006,10 +8005,10 @@
         <v>1.595</v>
       </c>
       <c r="B196">
-        <v>0.99999976810000002</v>
+        <v>0.99990713600000003</v>
       </c>
       <c r="C196" s="1">
-        <v>2.3189066590000001E-7</v>
+        <v>9.2864012010000007E-5</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -8017,10 +8016,10 @@
         <v>1.5960000000000001</v>
       </c>
       <c r="B197">
-        <v>0.99999976950000002</v>
+        <v>0.94071497439999996</v>
       </c>
       <c r="C197" s="1">
-        <v>2.3050258269999999E-7</v>
+        <v>5.9285025579999998E-2</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -8028,10 +8027,10 @@
         <v>1.597</v>
       </c>
       <c r="B198">
-        <v>0.99999976140000002</v>
+        <v>0.99990694270000002</v>
       </c>
       <c r="C198" s="1">
-        <v>2.3856224449999998E-7</v>
+        <v>9.3057257139999994E-5</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -8039,10 +8038,10 @@
         <v>1.5980000000000001</v>
       </c>
       <c r="B199">
-        <v>0.99999976960000003</v>
+        <v>0.99996097149999996</v>
       </c>
       <c r="C199" s="1">
-        <v>2.3044161690000001E-7</v>
+        <v>3.9028510250000001E-5</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -8050,10 +8049,10 @@
         <v>1.599</v>
       </c>
       <c r="B200">
-        <v>0.99999961410000004</v>
+        <v>0.99993301329999995</v>
       </c>
       <c r="C200" s="1">
-        <v>3.8585442329999999E-7</v>
+        <v>6.6986719140000003E-5</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -8061,10 +8060,10 @@
         <v>1.6</v>
       </c>
       <c r="B201">
-        <v>0.99999976950000002</v>
+        <v>0.57150331489999995</v>
       </c>
       <c r="C201" s="1">
-        <v>2.3045550620000001E-7</v>
+        <v>0.4284966851</v>
       </c>
     </row>
   </sheetData>
@@ -8077,7 +8076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Small changes to plots.
</commit_message>
<xml_diff>
--- a/ORR_Filter/ORR_Filter/Plots.xlsx
+++ b/ORR_Filter/ORR_Filter/Plots.xlsx
@@ -808,607 +808,607 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="431"/>
                 <c:pt idx="0">
-                  <c:v>0.99995939199999995</c:v>
+                  <c:v>0.9999694858</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99993383520000001</c:v>
+                  <c:v>0.99840731260000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.77410293770000005</c:v>
+                  <c:v>0.99997098390000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99992241299999995</c:v>
+                  <c:v>0.99926684450000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99996121770000002</c:v>
+                  <c:v>0.9999645049</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99994441359999997</c:v>
+                  <c:v>0.99993617170000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.99974407379999997</c:v>
+                  <c:v>0.99986842480000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99736309430000003</c:v>
+                  <c:v>0.99997074860000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.99986849560000002</c:v>
+                  <c:v>0.99976421380000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.99994212100000002</c:v>
+                  <c:v>0.99993292140000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99995769850000005</c:v>
+                  <c:v>0.99997016630000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.9999612859</c:v>
+                  <c:v>0.99983558989999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.99996074489999998</c:v>
+                  <c:v>0.99986959600000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.9999590236</c:v>
+                  <c:v>0.9999696763</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.9999579475</c:v>
+                  <c:v>0.99995686669999995</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.9999584064</c:v>
+                  <c:v>0.99918375429999995</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.99996002679999996</c:v>
+                  <c:v>0.99988810900000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.99996134579999996</c:v>
+                  <c:v>0.99996673390000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.99996006370000001</c:v>
+                  <c:v>0.99996903290000005</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.99995157499999998</c:v>
+                  <c:v>0.99993700090000004</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.9999175683</c:v>
+                  <c:v>0.99940298930000004</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.99964708719999995</c:v>
+                  <c:v>0.9995374896</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.99818933210000005</c:v>
+                  <c:v>0.99992625729999995</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.99990579670000002</c:v>
+                  <c:v>0.99996155340000004</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.99995857070000005</c:v>
+                  <c:v>0.99996987250000002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.99995400759999997</c:v>
+                  <c:v>0.99997078760000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.99976291019999997</c:v>
+                  <c:v>0.99996801899999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.99973956959999999</c:v>
+                  <c:v>0.99996280299999996</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.99995762479999994</c:v>
+                  <c:v>0.99995629180000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.99994062409999995</c:v>
+                  <c:v>0.99995036650000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.99132990649999997</c:v>
+                  <c:v>0.99994737580000004</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.99995297490000001</c:v>
+                  <c:v>0.99994874</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.99993490340000002</c:v>
+                  <c:v>0.99995378099999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.99960724459999994</c:v>
+                  <c:v>0.99996031210000003</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.99996138950000002</c:v>
+                  <c:v>0.99996618349999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.99932605240000005</c:v>
+                  <c:v>0.99997002550000003</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.99995355500000005</c:v>
+                  <c:v>0.99997082540000004</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.99985670550000005</c:v>
+                  <c:v>0.99996647000000005</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.99994336949999996</c:v>
+                  <c:v>0.99994816610000004</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.99987720889999998</c:v>
+                  <c:v>0.99984472049999995</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.99994859970000005</c:v>
+                  <c:v>0.65808237390000002</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.99973471020000004</c:v>
+                  <c:v>0.99987115849999997</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.99995991139999996</c:v>
+                  <c:v>0.99996073139999997</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.99117504190000005</c:v>
+                  <c:v>0.9999709161</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.9999550076</c:v>
+                  <c:v>0.99995192109999997</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.9999208758</c:v>
+                  <c:v>0.99931663959999995</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.99967705569999998</c:v>
+                  <c:v>0.99988378850000004</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.99996042439999999</c:v>
+                  <c:v>0.99996870019999995</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.99991328430000004</c:v>
+                  <c:v>0.99996032369999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.999102763</c:v>
+                  <c:v>0.99881293159999995</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.99995060499999999</c:v>
+                  <c:v>0.99993891109999999</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.99995700970000001</c:v>
+                  <c:v>0.99997034269999996</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.99982867379999996</c:v>
+                  <c:v>0.99982311199999996</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.99899775499999999</c:v>
+                  <c:v>0.99991859949999995</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.99992869419999997</c:v>
+                  <c:v>0.99997017359999996</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.99996014720000004</c:v>
+                  <c:v>0.99956179779999998</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.99995694830000004</c:v>
+                  <c:v>0.99995511869999998</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.9999248758</c:v>
+                  <c:v>0.99995760970000003</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.99976240149999995</c:v>
+                  <c:v>0.99969125270000003</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.99534515270000001</c:v>
+                  <c:v>0.99997085240000005</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.99869562150000002</c:v>
+                  <c:v>0.99827187780000004</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.99971262390000004</c:v>
+                  <c:v>0.99996859429999996</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.99984201130000006</c:v>
+                  <c:v>0.99979758029999999</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.99987834060000003</c:v>
+                  <c:v>0.99996434690000002</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.99988547520000004</c:v>
+                  <c:v>0.99985581759999997</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.99987161560000004</c:v>
+                  <c:v>0.99996479469999999</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.99981986720000005</c:v>
+                  <c:v>0.99976797750000002</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.99961508239999997</c:v>
+                  <c:v>0.99996924779999996</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.99638030180000003</c:v>
+                  <c:v>0.99520821209999999</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.99874250369999995</c:v>
+                  <c:v>0.99997048160000002</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.99984043690000002</c:v>
+                  <c:v>0.99979547449999995</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.99993818229999998</c:v>
+                  <c:v>0.99995198279999997</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.99995973400000004</c:v>
+                  <c:v>0.99996034180000004</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.99995744480000004</c:v>
+                  <c:v>0.99886880109999998</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.99990420369999999</c:v>
+                  <c:v>0.99996876899999998</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.98686493220000004</c:v>
+                  <c:v>0.99993721520000001</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.99989175109999995</c:v>
+                  <c:v>0.99968384229999996</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.99996009350000004</c:v>
+                  <c:v>0.99996900850000003</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.99994124350000002</c:v>
+                  <c:v>0.99994990969999997</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.99352246980000003</c:v>
+                  <c:v>0.99145705679999996</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.99993166779999998</c:v>
+                  <c:v>0.99995524199999997</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.99995863200000001</c:v>
+                  <c:v>0.99996984799999999</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.99944949370000002</c:v>
+                  <c:v>0.99990540949999995</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.99992962110000005</c:v>
+                  <c:v>0.99888319069999998</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.99995377259999996</c:v>
+                  <c:v>0.9999499731</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.99066593830000005</c:v>
+                  <c:v>0.99997091989999998</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.99995919779999998</c:v>
+                  <c:v>0.99995922820000005</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.99981659590000005</c:v>
+                  <c:v>0.99983338629999996</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.99993839920000005</c:v>
+                  <c:v>0.99721010450000003</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.99992293809999999</c:v>
+                  <c:v>0.99990641940000002</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.99991087670000001</c:v>
+                  <c:v>0.99996075309999999</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.99993363189999995</c:v>
+                  <c:v>0.99997044700000004</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.99991710739999995</c:v>
+                  <c:v>0.99996950240000004</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.99991143790000003</c:v>
+                  <c:v>0.99996065619999996</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.99994621019999996</c:v>
+                  <c:v>0.99993874289999995</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.99966765909999999</c:v>
+                  <c:v>0.99988535460000005</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.99996117100000004</c:v>
+                  <c:v>0.99973516890000003</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.99938248399999996</c:v>
+                  <c:v>0.99918508019999996</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.99994051989999999</c:v>
+                  <c:v>0.99594799990000005</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.99995017320000001</c:v>
+                  <c:v>0.94499560370000002</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.57150331489999995</c:v>
+                  <c:v>0.65808237390000002</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.99994686870000005</c:v>
+                  <c:v>0.94487242869999999</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.99995406050000002</c:v>
+                  <c:v>0.99592664109999995</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0.99937763820000003</c:v>
+                  <c:v>0.99917862999999996</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>0.99987996980000005</c:v>
+                  <c:v>0.99973244110000004</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>0.99996023020000002</c:v>
+                  <c:v>0.99988396310000005</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0.99994566080000002</c:v>
+                  <c:v>0.99993795399999996</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>0.99959974200000001</c:v>
+                  <c:v>0.99996019979999995</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>0.99960430280000001</c:v>
+                  <c:v>0.99996929879999996</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>0.99993653689999995</c:v>
+                  <c:v>0.99997059749999995</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>0.99996044139999996</c:v>
+                  <c:v>0.99996199149999998</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>0.9999574309</c:v>
+                  <c:v>0.99991589240000001</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>0.99993150590000002</c:v>
+                  <c:v>0.99870873719999997</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>0.99982656749999999</c:v>
+                  <c:v>0.99977693150000002</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>0.99888925210000001</c:v>
+                  <c:v>0.99995467189999998</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>0.99029413249999998</c:v>
+                  <c:v>0.99997092249999997</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>0.99940634719999999</c:v>
+                  <c:v>0.99995793249999998</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>0.99974394109999998</c:v>
+                  <c:v>0.99966662399999995</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>0.99982276569999995</c:v>
+                  <c:v>0.99982840449999999</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>0.99984274829999997</c:v>
+                  <c:v>0.99996618299999995</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>0.99983039819999997</c:v>
+                  <c:v>0.99996544750000005</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>0.99977044449999997</c:v>
+                  <c:v>0.99970198539999999</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>0.99954047619999997</c:v>
+                  <c:v>0.99989956030000005</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>0.99691584840000003</c:v>
+                  <c:v>0.99997078340000001</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>0.9974927039</c:v>
+                  <c:v>0.99992918760000005</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>0.99976055789999996</c:v>
+                  <c:v>0.9996887927</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>0.99991779179999996</c:v>
+                  <c:v>0.99996954220000001</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>0.99995362300000001</c:v>
+                  <c:v>0.99993199779999997</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>0.9999613678</c:v>
+                  <c:v>0.99981968619999995</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>0.9999485186</c:v>
+                  <c:v>0.99997098520000005</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>0.99982834939999998</c:v>
+                  <c:v>0.99977931330000003</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>0.99699477079999999</c:v>
+                  <c:v>0.99995050429999999</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>0.99992075130000002</c:v>
+                  <c:v>0.99995872330000002</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>0.99996108459999999</c:v>
+                  <c:v>0.99971906030000002</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>0.99993692850000004</c:v>
+                  <c:v>0.99997061700000001</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>0.99433581999999998</c:v>
+                  <c:v>0.99252126110000005</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>0.99992301920000004</c:v>
+                  <c:v>0.99996984639999997</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>0.99996069499999996</c:v>
+                  <c:v>0.99965340189999996</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>0.99980952609999996</c:v>
+                  <c:v>0.99996716699999999</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>0.99986259430000002</c:v>
+                  <c:v>0.99977683319999999</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>0.99996124710000001</c:v>
+                  <c:v>0.99996722589999998</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>0.99972547810000001</c:v>
+                  <c:v>0.99964199769999995</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>0.9999244008</c:v>
+                  <c:v>0.99996992669999996</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>0.99995229809999997</c:v>
+                  <c:v>0.99001765730000002</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>0.99854328469999998</c:v>
+                  <c:v>0.99997055199999996</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>0.99996116719999995</c:v>
+                  <c:v>0.99973442639999999</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>0.99943753319999995</c:v>
+                  <c:v>0.99995823409999995</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>0.99995449030000005</c:v>
+                  <c:v>0.99995109859999998</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>0.99982462729999999</c:v>
+                  <c:v>0.99977433849999997</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>0.99994867939999998</c:v>
+                  <c:v>0.99997098520000005</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>0.99983686230000002</c:v>
+                  <c:v>0.99981476329999996</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>0.99995286159999996</c:v>
+                  <c:v>0.99993403989999996</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>0.99962112759999999</c:v>
+                  <c:v>0.99996921790000004</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>0.99996043229999998</c:v>
+                  <c:v>0.99961013840000001</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>0.98980068929999998</c:v>
+                  <c:v>0.99993645419999999</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>0.99995693860000001</c:v>
+                  <c:v>0.99997035879999996</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>0.99989390909999998</c:v>
+                  <c:v>0.9998671562</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>0.99986242280000004</c:v>
+                  <c:v>0.99982489969999999</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>0.99996063859999995</c:v>
+                  <c:v>0.99996845300000003</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>0.99963125959999999</c:v>
+                  <c:v>0.99996068819999995</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>0.99991250210000004</c:v>
+                  <c:v>0.99949786799999996</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>0.99996041719999995</c:v>
+                  <c:v>0.99987952999999996</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>0.99980398339999998</c:v>
+                  <c:v>0.99996729309999999</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>0.99979377729999996</c:v>
+                  <c:v>0.99996750479999996</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>0.99995847090000001</c:v>
+                  <c:v>0.99990804950000001</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>0.99994779050000004</c:v>
+                  <c:v>0.84433625950000002</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>0.99948660180000004</c:v>
+                  <c:v>0.99990328740000001</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>0.99978001699999997</c:v>
+                  <c:v>0.99996384469999999</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>0.99995094679999996</c:v>
+                  <c:v>0.99997095560000004</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>0.9999607439</c:v>
+                  <c:v>0.99996281409999999</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>0.99993521490000004</c:v>
+                  <c:v>0.9999232736</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>0.99970333050000004</c:v>
+                  <c:v>0.99961246400000003</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>0.99585628079999999</c:v>
+                  <c:v>0.9945178898</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>0.99983951029999996</c:v>
+                  <c:v>0.9997942353</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>0.99993497539999998</c:v>
+                  <c:v>0.99992294179999996</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>0.99995548010000002</c:v>
+                  <c:v>0.99995268169999996</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>0.99996097589999999</c:v>
+                  <c:v>0.99996354249999997</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>0.99996084689999998</c:v>
+                  <c:v>0.99996815640000003</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>0.9999579072</c:v>
+                  <c:v>0.99997010419999999</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>0.99995378690000003</c:v>
+                  <c:v>0.99997080670000005</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>0.99995009619999997</c:v>
+                  <c:v>0.9999709739</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>0.99994836330000003</c:v>
+                  <c:v>0.99997098500000003</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>0.99994936420000002</c:v>
+                  <c:v>0.99997098240000004</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>0.99995263909999998</c:v>
+                  <c:v>0.99997088639999998</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>0.99995679429999995</c:v>
+                  <c:v>0.99997039030000001</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>0.99996021329999996</c:v>
+                  <c:v>0.99996890510000003</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>0.99996134759999999</c:v>
+                  <c:v>0.99996530819999996</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>0.99995802280000001</c:v>
+                  <c:v>0.99995700239999996</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>0.99994422189999999</c:v>
+                  <c:v>0.9999358988</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>0.99989001970000002</c:v>
+                  <c:v>0.99986192480000002</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>0.9993052067</c:v>
+                  <c:v>0.99908223169999999</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>0.99907871859999997</c:v>
+                  <c:v>0.99878095870000005</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>0.99990611190000001</c:v>
+                  <c:v>0.99988360320000003</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>0.99995658350000005</c:v>
+                  <c:v>0.99995450080000003</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>0.99995904459999996</c:v>
+                  <c:v>0.99996966629999995</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>0.99990713600000003</c:v>
+                  <c:v>0.99996893229999995</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>0.94071497439999996</c:v>
+                  <c:v>0.99994417440000005</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>0.99990694270000002</c:v>
+                  <c:v>0.99957004360000001</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>0.99996097149999996</c:v>
+                  <c:v>0.99969929930000001</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>0.99993301329999995</c:v>
+                  <c:v>0.99995466659999999</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>0.57150331489999995</c:v>
+                  <c:v>0.99997098520000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2054,607 +2054,607 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="431"/>
                 <c:pt idx="0">
-                  <c:v>4.0608006929999998E-5</c:v>
+                  <c:v>3.0514167520000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.6164787730000002E-5</c:v>
+                  <c:v>1.592687428E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22589706230000001</c:v>
+                  <c:v>2.9016056780000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.7586964230000002E-5</c:v>
+                  <c:v>7.3315553740000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8782293189999997E-5</c:v>
+                  <c:v>3.5495143800000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.5586431730000003E-5</c:v>
+                  <c:v>6.3828331170000005E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5592619869999999E-4</c:v>
+                  <c:v>1.315752227E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.6369057179999999E-3</c:v>
+                  <c:v>2.9251413109999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3150441149999999E-4</c:v>
+                  <c:v>2.3578616900000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.7879000499999997E-5</c:v>
+                  <c:v>6.7078587679999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.2301520619999999E-5</c:v>
+                  <c:v>2.9833686540000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.871409744E-5</c:v>
+                  <c:v>1.6441012219999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.9255064039999997E-5</c:v>
+                  <c:v>1.3040395319999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.0976381100000003E-5</c:v>
+                  <c:v>3.032369048E-5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.2052474260000002E-5</c:v>
+                  <c:v>4.3133296220000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.1593563580000003E-5</c:v>
+                  <c:v>8.1624570009999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.9973183370000003E-5</c:v>
+                  <c:v>1.118909837E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.8654200430000003E-5</c:v>
+                  <c:v>3.3266138859999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.9936312229999998E-5</c:v>
+                  <c:v>3.0967076860000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.8425036780000003E-5</c:v>
+                  <c:v>6.2999086670000005E-5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.2431701340000002E-5</c:v>
+                  <c:v>5.9701065079999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.5291283470000002E-4</c:v>
+                  <c:v>4.625104115E-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.8106678860000001E-3</c:v>
+                  <c:v>7.3742672629999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.4203291190000002E-5</c:v>
+                  <c:v>3.844658891E-5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.1429328869999998E-5</c:v>
+                  <c:v>3.012745978E-5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.5992363829999998E-5</c:v>
+                  <c:v>2.9212380370000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.370898474E-4</c:v>
+                  <c:v>3.198099096E-5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6043040009999998E-4</c:v>
+                  <c:v>3.719698337E-5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.2375247829999998E-5</c:v>
+                  <c:v>4.3708246869999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.9375938280000001E-5</c:v>
+                  <c:v>4.9633484259999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8.6700935429999994E-3</c:v>
+                  <c:v>5.2624209829999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.7025090339999998E-5</c:v>
+                  <c:v>5.1259991880000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.5096647460000003E-5</c:v>
+                  <c:v>4.6218961499999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.9275537929999999E-4</c:v>
+                  <c:v>3.9687927820000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.8610503850000003E-5</c:v>
+                  <c:v>3.3816492040000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.7394757440000005E-4</c:v>
+                  <c:v>2.9974479400000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.6445001069999998E-5</c:v>
+                  <c:v>2.9174593489999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.4329449630000001E-4</c:v>
+                  <c:v>3.353004491E-5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.6630522490000001E-5</c:v>
+                  <c:v>5.183385919E-5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.227910508E-4</c:v>
+                  <c:v>1.5527952490000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.1400267119999997E-5</c:v>
+                  <c:v>0.34191762609999998</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.6528976839999997E-4</c:v>
+                  <c:v>1.2884154790000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.0088576590000002E-5</c:v>
+                  <c:v>3.9268644200000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>8.8249581389999998E-3</c:v>
+                  <c:v>2.9083931690000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.499235362E-5</c:v>
+                  <c:v>4.8078885120000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>7.9124231799999995E-5</c:v>
+                  <c:v>6.8336042720000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.229442893E-4</c:v>
+                  <c:v>1.162114534E-4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.9575577929999999E-5</c:v>
+                  <c:v>3.1299822049999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>8.6715669049999998E-5</c:v>
+                  <c:v>3.967629254E-5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>8.9723696549999998E-4</c:v>
+                  <c:v>1.1870684340000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4.9394998649999997E-5</c:v>
+                  <c:v>6.1088948260000004E-5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.2990252659999998E-5</c:v>
+                  <c:v>2.9657255359999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.7132619090000001E-4</c:v>
+                  <c:v>1.7688798919999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.002244969E-3</c:v>
+                  <c:v>8.1400462799999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>7.1305785420000003E-5</c:v>
+                  <c:v>2.982635867E-5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3.9852756430000001E-5</c:v>
+                  <c:v>4.3820220660000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4.3051694829999999E-5</c:v>
+                  <c:v>4.4881344380000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>7.5124235449999999E-5</c:v>
+                  <c:v>4.2390331580000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.3759845809999999E-4</c:v>
+                  <c:v>3.0874728350000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4.6548472999999998E-3</c:v>
+                  <c:v>2.914757791E-5</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.3043784869999999E-3</c:v>
+                  <c:v>1.7281222250000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2.8737612249999999E-4</c:v>
+                  <c:v>3.1405706470000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.579886857E-4</c:v>
+                  <c:v>2.0241968389999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.216594168E-4</c:v>
+                  <c:v>3.5653058569999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.1452476710000001E-4</c:v>
+                  <c:v>1.4418241420000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.28384413E-4</c:v>
+                  <c:v>3.5205274460000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.8013280010000001E-4</c:v>
+                  <c:v>2.320225398E-4</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>3.8491758929999999E-4</c:v>
+                  <c:v>3.0752175529999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>3.6196981719999999E-3</c:v>
+                  <c:v>4.7917878719999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.257496343E-3</c:v>
+                  <c:v>2.9518442730000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.5956313800000001E-4</c:v>
+                  <c:v>2.0452549300000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>6.1817680940000005E-5</c:v>
+                  <c:v>4.8017239549999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>4.0265960210000001E-5</c:v>
+                  <c:v>3.965818874E-5</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>4.2555186469999999E-5</c:v>
+                  <c:v>1.1311989229999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>9.5796267729999997E-5</c:v>
+                  <c:v>3.1231006579999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1.313506777E-2</c:v>
+                  <c:v>6.2784832089999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1.0824894640000001E-4</c:v>
+                  <c:v>3.1615771569999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>3.9906541720000001E-5</c:v>
+                  <c:v>3.0991512489999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>5.8756486689999999E-5</c:v>
+                  <c:v>5.009031488E-5</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>6.4775301570000002E-3</c:v>
+                  <c:v>8.5429432069999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>6.8332177250000006E-5</c:v>
+                  <c:v>4.4758037769999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>4.1367956700000002E-5</c:v>
+                  <c:v>3.015198024E-5</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>5.5050625099999995E-4</c:v>
+                  <c:v>9.4590549470000004E-5</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>7.0378924260000006E-5</c:v>
+                  <c:v>1.1168092549999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4.6227376790000001E-5</c:v>
+                  <c:v>5.0026854559999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>9.3340617389999995E-3</c:v>
+                  <c:v>2.9080068230000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>4.080221217E-5</c:v>
+                  <c:v>4.0771793000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.8340414600000001E-4</c:v>
+                  <c:v>1.6661366800000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>6.1600821439999998E-5</c:v>
+                  <c:v>2.7898955029999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>7.7061856030000004E-5</c:v>
+                  <c:v>9.358058997E-5</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>8.9123311180000001E-5</c:v>
+                  <c:v>3.9246859139999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>6.6368127200000003E-5</c:v>
+                  <c:v>2.9552976190000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>8.2892625919999999E-5</c:v>
+                  <c:v>3.0497586009999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>8.8562148310000006E-5</c:v>
+                  <c:v>3.9343785740000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>5.378976086E-5</c:v>
+                  <c:v>6.125708129E-5</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>3.3234086359999998E-4</c:v>
+                  <c:v>1.146454167E-4</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>3.8829012670000002E-5</c:v>
+                  <c:v>2.6483108060000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>6.1751595630000003E-4</c:v>
+                  <c:v>8.1491981630000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>5.94801035E-5</c:v>
+                  <c:v>4.0520000779999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>4.9826769390000001E-5</c:v>
+                  <c:v>5.5004396259999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.4284966851</c:v>
+                  <c:v>0.34191762609999998</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>5.3131317670000002E-5</c:v>
+                  <c:v>5.5127571290000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>4.593946118E-5</c:v>
+                  <c:v>4.0733589030000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>6.2236176299999997E-4</c:v>
+                  <c:v>8.213699631E-4</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1.200302451E-4</c:v>
+                  <c:v>2.675589033E-4</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>3.9769848569999998E-5</c:v>
+                  <c:v>1.16036857E-4</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>5.4339213339999999E-5</c:v>
+                  <c:v>6.2045982289999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>4.0025799429999997E-4</c:v>
+                  <c:v>3.9800154720000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>3.9569715030000001E-4</c:v>
+                  <c:v>3.070122954E-5</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>6.3463143110000005E-5</c:v>
+                  <c:v>2.9402468980000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>3.9558598330000003E-5</c:v>
+                  <c:v>3.8008530950000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>4.2569108459999999E-5</c:v>
+                  <c:v>8.4107563829999995E-5</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>6.8494124189999998E-5</c:v>
+                  <c:v>1.291262836E-3</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1.7343253359999999E-4</c:v>
+                  <c:v>2.230684732E-4</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1.1107479070000001E-3</c:v>
+                  <c:v>4.532807493E-5</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>9.7058675489999999E-3</c:v>
+                  <c:v>2.90775035E-5</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>5.9365283949999997E-4</c:v>
+                  <c:v>4.206754673E-5</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>2.5605885190000001E-4</c:v>
+                  <c:v>3.3337604589999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>1.7723428050000001E-4</c:v>
+                  <c:v>1.7159553780000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>1.572517208E-4</c:v>
+                  <c:v>3.3816966850000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>1.6960184250000001E-4</c:v>
+                  <c:v>3.4552549430000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>2.2955551850000001E-4</c:v>
+                  <c:v>2.9801462560000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>4.595237992E-4</c:v>
+                  <c:v>1.004397467E-4</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>3.0841516299999999E-3</c:v>
+                  <c:v>2.921657398E-5</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>2.5072960509999998E-3</c:v>
+                  <c:v>7.0812437879999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>2.3944214650000001E-4</c:v>
+                  <c:v>3.1120733409999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>8.22081809E-5</c:v>
+                  <c:v>3.0457844179999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>4.637698821E-5</c:v>
+                  <c:v>6.8002183890000006E-5</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>3.8632215389999997E-5</c:v>
+                  <c:v>1.803138484E-4</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>5.1481385129999998E-5</c:v>
+                  <c:v>2.901478644E-5</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>1.7165058499999999E-4</c:v>
+                  <c:v>2.2068671679999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>3.0052292049999999E-3</c:v>
+                  <c:v>4.9495703120000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>7.9248652110000003E-5</c:v>
+                  <c:v>4.1276718580000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>3.8915431740000002E-5</c:v>
+                  <c:v>2.8093972549999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>6.3071473739999994E-5</c:v>
+                  <c:v>2.9383041240000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>5.6641800080000004E-3</c:v>
+                  <c:v>7.478738853E-3</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>7.6980817890000001E-5</c:v>
+                  <c:v>3.0153557780000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>3.9304988819999997E-5</c:v>
+                  <c:v>3.4659812839999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>1.904738684E-4</c:v>
+                  <c:v>3.2833021240000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>1.3740569449999999E-4</c:v>
+                  <c:v>2.231668349E-4</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>3.8752937859999999E-5</c:v>
+                  <c:v>3.2774086589999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>2.7452194129999998E-4</c:v>
+                  <c:v>3.5800225010000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>7.5599163030000001E-5</c:v>
+                  <c:v>3.0073287269999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>4.770191941E-5</c:v>
+                  <c:v>9.9823426950000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>1.4567152800000001E-3</c:v>
+                  <c:v>2.9448030789999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>3.8832843970000003E-5</c:v>
+                  <c:v>2.6557358840000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>5.6246680240000003E-4</c:v>
+                  <c:v>4.176590091E-5</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>4.5509734060000001E-5</c:v>
+                  <c:v>4.8901400300000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>1.7537272560000001E-4</c:v>
+                  <c:v>2.2566153869999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>5.1320573069999999E-5</c:v>
+                  <c:v>2.901478566E-5</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>1.6313768640000001E-4</c:v>
+                  <c:v>1.852367077E-4</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>4.7138380119999999E-5</c:v>
+                  <c:v>6.5960127939999996E-5</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>3.7887237270000003E-4</c:v>
+                  <c:v>3.0782116049999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>3.9567738049999997E-5</c:v>
+                  <c:v>3.898616369E-4</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>1.01993107E-2</c:v>
+                  <c:v>6.3545765880000006E-5</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>4.3061404710000003E-5</c:v>
+                  <c:v>2.9641201300000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>1.060908947E-4</c:v>
+                  <c:v>1.3284383790000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>1.3757724960000001E-4</c:v>
+                  <c:v>1.7510027889999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>3.936141365E-5</c:v>
+                  <c:v>3.1547031300000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>3.687403763E-4</c:v>
+                  <c:v>3.931182152E-5</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>8.7497919250000006E-5</c:v>
+                  <c:v>5.0213195979999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>3.9582835309999997E-5</c:v>
+                  <c:v>1.2047001949999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>1.9601663139999999E-4</c:v>
+                  <c:v>3.2706878379999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>2.0622267300000001E-4</c:v>
+                  <c:v>3.2495191780000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>4.1529124099999999E-5</c:v>
+                  <c:v>9.1950549569999994E-5</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>5.2209521510000001E-5</c:v>
+                  <c:v>0.15566374050000001</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>5.133981914E-4</c:v>
+                  <c:v>9.6712576790000004E-5</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>2.199829933E-4</c:v>
+                  <c:v>3.6155263979999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>4.9053235049999998E-5</c:v>
+                  <c:v>2.9044354659999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>3.9256098470000002E-5</c:v>
+                  <c:v>3.7185872150000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>6.4785090479999995E-5</c:v>
+                  <c:v>7.672638482E-5</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>2.9666945419999999E-4</c:v>
+                  <c:v>3.8753598770000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>4.1437191959999998E-3</c:v>
+                  <c:v>5.4821101889999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>1.6048974050000001E-4</c:v>
+                  <c:v>2.0576472740000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>6.5024635949999997E-5</c:v>
+                  <c:v>7.7058176460000007E-5</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>4.4519864950000002E-5</c:v>
+                  <c:v>4.7318298039999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>3.9024149390000002E-5</c:v>
+                  <c:v>3.6457535699999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>3.915310307E-5</c:v>
+                  <c:v>3.1843615000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>4.2092825300000001E-5</c:v>
+                  <c:v>2.989579762E-5</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>4.62130988E-5</c:v>
+                  <c:v>2.9193259359999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>4.9903782309999997E-5</c:v>
+                  <c:v>2.9026138249999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>5.1636682540000001E-5</c:v>
+                  <c:v>2.9015011769999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>5.0635785890000001E-5</c:v>
+                  <c:v>2.9017593860000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>4.7360860229999999E-5</c:v>
+                  <c:v>2.9113634359999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>4.3205692569999997E-5</c:v>
+                  <c:v>2.9609749110000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>3.9786667470000001E-5</c:v>
+                  <c:v>3.1094900589999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>3.865239457E-5</c:v>
+                  <c:v>3.4691801950000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>4.1977195429999997E-5</c:v>
+                  <c:v>4.2997555740000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>5.577806606E-5</c:v>
+                  <c:v>6.4101234409999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>1.0998034610000001E-4</c:v>
+                  <c:v>1.3807522419999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>6.947933288E-4</c:v>
+                  <c:v>9.177683069E-4</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>9.2128142779999999E-4</c:v>
+                  <c:v>1.2190412749999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>9.3888100980000003E-5</c:v>
+                  <c:v>1.163967931E-4</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>4.3416544190000001E-5</c:v>
+                  <c:v>4.5499182759999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>4.0955429520000001E-5</c:v>
+                  <c:v>3.0333700089999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>9.2864012010000007E-5</c:v>
+                  <c:v>3.1067680030000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>5.9285025579999998E-2</c:v>
+                  <c:v>5.5825575320000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>9.3057257139999994E-5</c:v>
+                  <c:v>4.2995643059999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>3.9028510250000001E-5</c:v>
+                  <c:v>3.0070073399999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>6.6986719140000003E-5</c:v>
+                  <c:v>4.5333362249999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>0.4284966851</c:v>
+                  <c:v>2.9014756060000001E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5832,17 +5832,17 @@
         <v>1.4</v>
       </c>
       <c r="B1">
-        <v>0.99995939199999995</v>
+        <v>0.9999694858</v>
       </c>
       <c r="C1" s="1">
-        <v>4.0608006929999998E-5</v>
+        <v>3.0514167520000001E-5</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2">
         <f>MAX(B1:B201)</f>
-        <v>0.99996138950000002</v>
+        <v>0.99997098520000005</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5850,17 +5850,17 @@
         <v>1.401</v>
       </c>
       <c r="B2">
-        <v>0.99993383520000001</v>
+        <v>0.99840731260000004</v>
       </c>
       <c r="C2" s="1">
-        <v>6.6164787730000002E-5</v>
+        <v>1.592687428E-3</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2">
         <f>MIN(B1:B201)</f>
-        <v>0.57150331489999995</v>
+        <v>0.65808237390000002</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5868,17 +5868,17 @@
         <v>1.4019999999999999</v>
       </c>
       <c r="B3">
-        <v>0.77410293770000005</v>
+        <v>0.99997098390000005</v>
       </c>
       <c r="C3" s="1">
-        <v>0.22589706230000001</v>
+        <v>2.9016056780000001E-5</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="2">
         <f>MAX(C1:C201)</f>
-        <v>0.4284966851</v>
+        <v>0.34191762609999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5886,17 +5886,17 @@
         <v>1.403</v>
       </c>
       <c r="B4">
-        <v>0.99992241299999995</v>
+        <v>0.99926684450000003</v>
       </c>
       <c r="C4" s="1">
-        <v>7.7586964230000002E-5</v>
+        <v>7.3315553740000003E-4</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="2">
         <f>MIN(C1:C204)</f>
-        <v>3.8610503850000003E-5</v>
+        <v>2.9014756060000001E-5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5904,10 +5904,10 @@
         <v>1.4039999999999999</v>
       </c>
       <c r="B5">
-        <v>0.99996121770000002</v>
+        <v>0.9999645049</v>
       </c>
       <c r="C5" s="1">
-        <v>3.8782293189999997E-5</v>
+        <v>3.5495143800000002E-5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -5915,10 +5915,10 @@
         <v>1.405</v>
       </c>
       <c r="B6">
-        <v>0.99994441359999997</v>
+        <v>0.99993617170000004</v>
       </c>
       <c r="C6" s="1">
-        <v>5.5586431730000003E-5</v>
+        <v>6.3828331170000005E-5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -5926,10 +5926,10 @@
         <v>1.4059999999999999</v>
       </c>
       <c r="B7">
-        <v>0.99974407379999997</v>
+        <v>0.99986842480000004</v>
       </c>
       <c r="C7" s="1">
-        <v>2.5592619869999999E-4</v>
+        <v>1.315752227E-4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -5937,10 +5937,10 @@
         <v>1.407</v>
       </c>
       <c r="B8">
-        <v>0.99736309430000003</v>
+        <v>0.99997074860000001</v>
       </c>
       <c r="C8" s="1">
-        <v>2.6369057179999999E-3</v>
+        <v>2.9251413109999999E-5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -5948,10 +5948,10 @@
         <v>1.4079999999999999</v>
       </c>
       <c r="B9">
-        <v>0.99986849560000002</v>
+        <v>0.99976421380000002</v>
       </c>
       <c r="C9" s="1">
-        <v>1.3150441149999999E-4</v>
+        <v>2.3578616900000001E-4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -5959,10 +5959,10 @@
         <v>1.409</v>
       </c>
       <c r="B10">
-        <v>0.99994212100000002</v>
+        <v>0.99993292140000001</v>
       </c>
       <c r="C10" s="1">
-        <v>5.7879000499999997E-5</v>
+        <v>6.7078587679999998E-5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -5970,10 +5970,10 @@
         <v>1.41</v>
       </c>
       <c r="B11">
-        <v>0.99995769850000005</v>
+        <v>0.99997016630000002</v>
       </c>
       <c r="C11" s="1">
-        <v>4.2301520619999999E-5</v>
+        <v>2.9833686540000001E-5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -5981,10 +5981,10 @@
         <v>1.411</v>
       </c>
       <c r="B12">
-        <v>0.9999612859</v>
+        <v>0.99983558989999999</v>
       </c>
       <c r="C12" s="1">
-        <v>3.871409744E-5</v>
+        <v>1.6441012219999999E-4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -5992,10 +5992,10 @@
         <v>1.4119999999999999</v>
       </c>
       <c r="B13">
-        <v>0.99996074489999998</v>
+        <v>0.99986959600000003</v>
       </c>
       <c r="C13" s="1">
-        <v>3.9255064039999997E-5</v>
+        <v>1.3040395319999999E-4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6003,10 +6003,10 @@
         <v>1.413</v>
       </c>
       <c r="B14">
-        <v>0.9999590236</v>
+        <v>0.9999696763</v>
       </c>
       <c r="C14" s="1">
-        <v>4.0976381100000003E-5</v>
+        <v>3.032369048E-5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -6014,10 +6014,10 @@
         <v>1.4139999999999999</v>
       </c>
       <c r="B15">
-        <v>0.9999579475</v>
+        <v>0.99995686669999995</v>
       </c>
       <c r="C15" s="1">
-        <v>4.2052474260000002E-5</v>
+        <v>4.3133296220000001E-5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -6025,10 +6025,10 @@
         <v>1.415</v>
       </c>
       <c r="B16">
-        <v>0.9999584064</v>
+        <v>0.99918375429999995</v>
       </c>
       <c r="C16" s="1">
-        <v>4.1593563580000003E-5</v>
+        <v>8.1624570009999995E-4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -6036,10 +6036,10 @@
         <v>1.4159999999999999</v>
       </c>
       <c r="B17">
-        <v>0.99996002679999996</v>
+        <v>0.99988810900000002</v>
       </c>
       <c r="C17" s="1">
-        <v>3.9973183370000003E-5</v>
+        <v>1.118909837E-4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6047,10 +6047,10 @@
         <v>1.417</v>
       </c>
       <c r="B18">
-        <v>0.99996134579999996</v>
+        <v>0.99996673390000002</v>
       </c>
       <c r="C18" s="1">
-        <v>3.8654200430000003E-5</v>
+        <v>3.3266138859999999E-5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6058,10 +6058,10 @@
         <v>1.4179999999999999</v>
       </c>
       <c r="B19">
-        <v>0.99996006370000001</v>
+        <v>0.99996903290000005</v>
       </c>
       <c r="C19" s="1">
-        <v>3.9936312229999998E-5</v>
+        <v>3.0967076860000003E-5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6069,10 +6069,10 @@
         <v>1.419</v>
       </c>
       <c r="B20">
-        <v>0.99995157499999998</v>
+        <v>0.99993700090000004</v>
       </c>
       <c r="C20" s="1">
-        <v>4.8425036780000003E-5</v>
+        <v>6.2999086670000005E-5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -6080,10 +6080,10 @@
         <v>1.42</v>
       </c>
       <c r="B21">
-        <v>0.9999175683</v>
+        <v>0.99940298930000004</v>
       </c>
       <c r="C21" s="1">
-        <v>8.2431701340000002E-5</v>
+        <v>5.9701065079999997E-4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6091,10 +6091,10 @@
         <v>1.421</v>
       </c>
       <c r="B22">
-        <v>0.99964708719999995</v>
+        <v>0.9995374896</v>
       </c>
       <c r="C22" s="1">
-        <v>3.5291283470000002E-4</v>
+        <v>4.625104115E-4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -6102,10 +6102,10 @@
         <v>1.4219999999999999</v>
       </c>
       <c r="B23">
-        <v>0.99818933210000005</v>
+        <v>0.99992625729999995</v>
       </c>
       <c r="C23" s="1">
-        <v>1.8106678860000001E-3</v>
+        <v>7.3742672629999997E-5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6113,10 +6113,10 @@
         <v>1.423</v>
       </c>
       <c r="B24">
-        <v>0.99990579670000002</v>
+        <v>0.99996155340000004</v>
       </c>
       <c r="C24" s="1">
-        <v>9.4203291190000002E-5</v>
+        <v>3.844658891E-5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -6124,10 +6124,10 @@
         <v>1.4239999999999999</v>
       </c>
       <c r="B25">
-        <v>0.99995857070000005</v>
+        <v>0.99996987250000002</v>
       </c>
       <c r="C25" s="1">
-        <v>4.1429328869999998E-5</v>
+        <v>3.012745978E-5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -6135,10 +6135,10 @@
         <v>1.425</v>
       </c>
       <c r="B26">
-        <v>0.99995400759999997</v>
+        <v>0.99997078760000002</v>
       </c>
       <c r="C26" s="1">
-        <v>4.5992363829999998E-5</v>
+        <v>2.9212380370000001E-5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -6146,10 +6146,10 @@
         <v>1.4259999999999999</v>
       </c>
       <c r="B27">
-        <v>0.99976291019999997</v>
+        <v>0.99996801899999999</v>
       </c>
       <c r="C27" s="1">
-        <v>2.370898474E-4</v>
+        <v>3.198099096E-5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -6157,10 +6157,10 @@
         <v>1.427</v>
       </c>
       <c r="B28">
-        <v>0.99973956959999999</v>
+        <v>0.99996280299999996</v>
       </c>
       <c r="C28" s="1">
-        <v>2.6043040009999998E-4</v>
+        <v>3.719698337E-5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -6168,10 +6168,10 @@
         <v>1.4279999999999999</v>
       </c>
       <c r="B29">
-        <v>0.99995762479999994</v>
+        <v>0.99995629180000001</v>
       </c>
       <c r="C29" s="1">
-        <v>4.2375247829999998E-5</v>
+        <v>4.3708246869999997E-5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -6179,10 +6179,10 @@
         <v>1.429</v>
       </c>
       <c r="B30">
-        <v>0.99994062409999995</v>
+        <v>0.99995036650000002</v>
       </c>
       <c r="C30" s="1">
-        <v>5.9375938280000001E-5</v>
+        <v>4.9633484259999997E-5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -6190,10 +6190,10 @@
         <v>1.43</v>
       </c>
       <c r="B31">
-        <v>0.99132990649999997</v>
+        <v>0.99994737580000004</v>
       </c>
       <c r="C31" s="1">
-        <v>8.6700935429999994E-3</v>
+        <v>5.2624209829999997E-5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -6201,10 +6201,10 @@
         <v>1.431</v>
       </c>
       <c r="B32">
-        <v>0.99995297490000001</v>
+        <v>0.99994874</v>
       </c>
       <c r="C32" s="1">
-        <v>4.7025090339999998E-5</v>
+        <v>5.1259991880000001E-5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6212,10 +6212,10 @@
         <v>1.4319999999999999</v>
       </c>
       <c r="B33">
-        <v>0.99993490340000002</v>
+        <v>0.99995378099999999</v>
       </c>
       <c r="C33" s="1">
-        <v>6.5096647460000003E-5</v>
+        <v>4.6218961499999997E-5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6223,10 +6223,10 @@
         <v>1.4330000000000001</v>
       </c>
       <c r="B34">
-        <v>0.99960724459999994</v>
+        <v>0.99996031210000003</v>
       </c>
       <c r="C34" s="1">
-        <v>3.9275537929999999E-4</v>
+        <v>3.9687927820000003E-5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6234,10 +6234,10 @@
         <v>1.4339999999999999</v>
       </c>
       <c r="B35">
-        <v>0.99996138950000002</v>
+        <v>0.99996618349999999</v>
       </c>
       <c r="C35" s="1">
-        <v>3.8610503850000003E-5</v>
+        <v>3.3816492040000001E-5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -6245,10 +6245,10 @@
         <v>1.4350000000000001</v>
       </c>
       <c r="B36">
-        <v>0.99932605240000005</v>
+        <v>0.99997002550000003</v>
       </c>
       <c r="C36" s="1">
-        <v>6.7394757440000005E-4</v>
+        <v>2.9974479400000001E-5</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6256,10 +6256,10 @@
         <v>1.4359999999999999</v>
       </c>
       <c r="B37">
-        <v>0.99995355500000005</v>
+        <v>0.99997082540000004</v>
       </c>
       <c r="C37" s="1">
-        <v>4.6445001069999998E-5</v>
+        <v>2.9174593489999999E-5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -6267,10 +6267,10 @@
         <v>1.4370000000000001</v>
       </c>
       <c r="B38">
-        <v>0.99985670550000005</v>
+        <v>0.99996647000000005</v>
       </c>
       <c r="C38" s="1">
-        <v>1.4329449630000001E-4</v>
+        <v>3.353004491E-5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -6278,10 +6278,10 @@
         <v>1.4379999999999999</v>
       </c>
       <c r="B39">
-        <v>0.99994336949999996</v>
+        <v>0.99994816610000004</v>
       </c>
       <c r="C39" s="1">
-        <v>5.6630522490000001E-5</v>
+        <v>5.183385919E-5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -6289,10 +6289,10 @@
         <v>1.4390000000000001</v>
       </c>
       <c r="B40">
-        <v>0.99987720889999998</v>
+        <v>0.99984472049999995</v>
       </c>
       <c r="C40" s="1">
-        <v>1.227910508E-4</v>
+        <v>1.5527952490000001E-4</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -6300,10 +6300,10 @@
         <v>1.44</v>
       </c>
       <c r="B41">
-        <v>0.99994859970000005</v>
+        <v>0.65808237390000002</v>
       </c>
       <c r="C41" s="1">
-        <v>5.1400267119999997E-5</v>
+        <v>0.34191762609999998</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6311,10 +6311,10 @@
         <v>1.4410000000000001</v>
       </c>
       <c r="B42">
-        <v>0.99973471020000004</v>
+        <v>0.99987115849999997</v>
       </c>
       <c r="C42" s="1">
-        <v>2.6528976839999997E-4</v>
+        <v>1.2884154790000001E-4</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -6322,10 +6322,10 @@
         <v>1.4419999999999999</v>
       </c>
       <c r="B43">
-        <v>0.99995991139999996</v>
+        <v>0.99996073139999997</v>
       </c>
       <c r="C43" s="1">
-        <v>4.0088576590000002E-5</v>
+        <v>3.9268644200000002E-5</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -6333,10 +6333,10 @@
         <v>1.4430000000000001</v>
       </c>
       <c r="B44">
-        <v>0.99117504190000005</v>
+        <v>0.9999709161</v>
       </c>
       <c r="C44" s="1">
-        <v>8.8249581389999998E-3</v>
+        <v>2.9083931690000001E-5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -6344,10 +6344,10 @@
         <v>1.444</v>
       </c>
       <c r="B45">
-        <v>0.9999550076</v>
+        <v>0.99995192109999997</v>
       </c>
       <c r="C45" s="1">
-        <v>4.499235362E-5</v>
+        <v>4.8078885120000002E-5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -6355,10 +6355,10 @@
         <v>1.4450000000000001</v>
       </c>
       <c r="B46">
-        <v>0.9999208758</v>
+        <v>0.99931663959999995</v>
       </c>
       <c r="C46" s="1">
-        <v>7.9124231799999995E-5</v>
+        <v>6.8336042720000003E-4</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -6366,10 +6366,10 @@
         <v>1.446</v>
       </c>
       <c r="B47">
-        <v>0.99967705569999998</v>
+        <v>0.99988378850000004</v>
       </c>
       <c r="C47" s="1">
-        <v>3.229442893E-4</v>
+        <v>1.162114534E-4</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6377,10 +6377,10 @@
         <v>1.4470000000000001</v>
       </c>
       <c r="B48">
-        <v>0.99996042439999999</v>
+        <v>0.99996870019999995</v>
       </c>
       <c r="C48" s="1">
-        <v>3.9575577929999999E-5</v>
+        <v>3.1299822049999997E-5</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -6388,10 +6388,10 @@
         <v>1.448</v>
       </c>
       <c r="B49">
-        <v>0.99991328430000004</v>
+        <v>0.99996032369999999</v>
       </c>
       <c r="C49" s="1">
-        <v>8.6715669049999998E-5</v>
+        <v>3.967629254E-5</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -6399,10 +6399,10 @@
         <v>1.4490000000000001</v>
       </c>
       <c r="B50">
-        <v>0.999102763</v>
+        <v>0.99881293159999995</v>
       </c>
       <c r="C50" s="1">
-        <v>8.9723696549999998E-4</v>
+        <v>1.1870684340000001E-3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -6410,10 +6410,10 @@
         <v>1.45</v>
       </c>
       <c r="B51">
-        <v>0.99995060499999999</v>
+        <v>0.99993891109999999</v>
       </c>
       <c r="C51" s="1">
-        <v>4.9394998649999997E-5</v>
+        <v>6.1088948260000004E-5</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -6421,10 +6421,10 @@
         <v>1.4510000000000001</v>
       </c>
       <c r="B52">
-        <v>0.99995700970000001</v>
+        <v>0.99997034269999996</v>
       </c>
       <c r="C52" s="1">
-        <v>4.2990252659999998E-5</v>
+        <v>2.9657255359999999E-5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -6432,10 +6432,10 @@
         <v>1.452</v>
       </c>
       <c r="B53">
-        <v>0.99982867379999996</v>
+        <v>0.99982311199999996</v>
       </c>
       <c r="C53" s="1">
-        <v>1.7132619090000001E-4</v>
+        <v>1.7688798919999999E-4</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -6443,10 +6443,10 @@
         <v>1.4530000000000001</v>
       </c>
       <c r="B54">
-        <v>0.99899775499999999</v>
+        <v>0.99991859949999995</v>
       </c>
       <c r="C54" s="1">
-        <v>1.002244969E-3</v>
+        <v>8.1400462799999997E-5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -6454,10 +6454,10 @@
         <v>1.454</v>
       </c>
       <c r="B55">
-        <v>0.99992869419999997</v>
+        <v>0.99997017359999996</v>
       </c>
       <c r="C55" s="1">
-        <v>7.1305785420000003E-5</v>
+        <v>2.982635867E-5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -6465,10 +6465,10 @@
         <v>1.4550000000000001</v>
       </c>
       <c r="B56">
-        <v>0.99996014720000004</v>
+        <v>0.99956179779999998</v>
       </c>
       <c r="C56" s="1">
-        <v>3.9852756430000001E-5</v>
+        <v>4.3820220660000002E-4</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -6476,10 +6476,10 @@
         <v>1.456</v>
       </c>
       <c r="B57">
-        <v>0.99995694830000004</v>
+        <v>0.99995511869999998</v>
       </c>
       <c r="C57" s="1">
-        <v>4.3051694829999999E-5</v>
+        <v>4.4881344380000001E-5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -6487,10 +6487,10 @@
         <v>1.4570000000000001</v>
       </c>
       <c r="B58">
-        <v>0.9999248758</v>
+        <v>0.99995760970000003</v>
       </c>
       <c r="C58" s="1">
-        <v>7.5124235449999999E-5</v>
+        <v>4.2390331580000001E-5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -6498,10 +6498,10 @@
         <v>1.458</v>
       </c>
       <c r="B59">
-        <v>0.99976240149999995</v>
+        <v>0.99969125270000003</v>
       </c>
       <c r="C59" s="1">
-        <v>2.3759845809999999E-4</v>
+        <v>3.0874728350000001E-4</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -6509,10 +6509,10 @@
         <v>1.4590000000000001</v>
       </c>
       <c r="B60">
-        <v>0.99534515270000001</v>
+        <v>0.99997085240000005</v>
       </c>
       <c r="C60" s="1">
-        <v>4.6548472999999998E-3</v>
+        <v>2.914757791E-5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -6520,10 +6520,10 @@
         <v>1.46</v>
       </c>
       <c r="B61">
-        <v>0.99869562150000002</v>
+        <v>0.99827187780000004</v>
       </c>
       <c r="C61" s="1">
-        <v>1.3043784869999999E-3</v>
+        <v>1.7281222250000001E-3</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -6531,10 +6531,10 @@
         <v>1.4610000000000001</v>
       </c>
       <c r="B62">
-        <v>0.99971262390000004</v>
+        <v>0.99996859429999996</v>
       </c>
       <c r="C62" s="1">
-        <v>2.8737612249999999E-4</v>
+        <v>3.1405706470000002E-5</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -6542,10 +6542,10 @@
         <v>1.462</v>
       </c>
       <c r="B63">
-        <v>0.99984201130000006</v>
+        <v>0.99979758029999999</v>
       </c>
       <c r="C63" s="1">
-        <v>1.579886857E-4</v>
+        <v>2.0241968389999999E-4</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -6553,10 +6553,10 @@
         <v>1.4630000000000001</v>
       </c>
       <c r="B64">
-        <v>0.99987834060000003</v>
+        <v>0.99996434690000002</v>
       </c>
       <c r="C64" s="1">
-        <v>1.216594168E-4</v>
+        <v>3.5653058569999998E-5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -6564,10 +6564,10 @@
         <v>1.464</v>
       </c>
       <c r="B65">
-        <v>0.99988547520000004</v>
+        <v>0.99985581759999997</v>
       </c>
       <c r="C65" s="1">
-        <v>1.1452476710000001E-4</v>
+        <v>1.4418241420000001E-4</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -6575,10 +6575,10 @@
         <v>1.4650000000000001</v>
       </c>
       <c r="B66">
-        <v>0.99987161560000004</v>
+        <v>0.99996479469999999</v>
       </c>
       <c r="C66" s="1">
-        <v>1.28384413E-4</v>
+        <v>3.5205274460000001E-5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6586,10 +6586,10 @@
         <v>1.466</v>
       </c>
       <c r="B67">
-        <v>0.99981986720000005</v>
+        <v>0.99976797750000002</v>
       </c>
       <c r="C67" s="1">
-        <v>1.8013280010000001E-4</v>
+        <v>2.320225398E-4</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -6597,10 +6597,10 @@
         <v>1.4670000000000001</v>
       </c>
       <c r="B68">
-        <v>0.99961508239999997</v>
+        <v>0.99996924779999996</v>
       </c>
       <c r="C68" s="1">
-        <v>3.8491758929999999E-4</v>
+        <v>3.0752175529999999E-5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -6608,10 +6608,10 @@
         <v>1.468</v>
       </c>
       <c r="B69">
-        <v>0.99638030180000003</v>
+        <v>0.99520821209999999</v>
       </c>
       <c r="C69" s="1">
-        <v>3.6196981719999999E-3</v>
+        <v>4.7917878719999996E-3</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6619,10 +6619,10 @@
         <v>1.4690000000000001</v>
       </c>
       <c r="B70">
-        <v>0.99874250369999995</v>
+        <v>0.99997048160000002</v>
       </c>
       <c r="C70" s="1">
-        <v>1.257496343E-3</v>
+        <v>2.9518442730000001E-5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -6630,10 +6630,10 @@
         <v>1.47</v>
       </c>
       <c r="B71">
-        <v>0.99984043690000002</v>
+        <v>0.99979547449999995</v>
       </c>
       <c r="C71" s="1">
-        <v>1.5956313800000001E-4</v>
+        <v>2.0452549300000001E-4</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -6641,10 +6641,10 @@
         <v>1.4710000000000001</v>
       </c>
       <c r="B72">
-        <v>0.99993818229999998</v>
+        <v>0.99995198279999997</v>
       </c>
       <c r="C72" s="1">
-        <v>6.1817680940000005E-5</v>
+        <v>4.8017239549999999E-5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -6652,10 +6652,10 @@
         <v>1.472</v>
       </c>
       <c r="B73">
-        <v>0.99995973400000004</v>
+        <v>0.99996034180000004</v>
       </c>
       <c r="C73" s="1">
-        <v>4.0265960210000001E-5</v>
+        <v>3.965818874E-5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6663,10 +6663,10 @@
         <v>1.4730000000000001</v>
       </c>
       <c r="B74">
-        <v>0.99995744480000004</v>
+        <v>0.99886880109999998</v>
       </c>
       <c r="C74" s="1">
-        <v>4.2555186469999999E-5</v>
+        <v>1.1311989229999999E-3</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -6674,10 +6674,10 @@
         <v>1.474</v>
       </c>
       <c r="B75">
-        <v>0.99990420369999999</v>
+        <v>0.99996876899999998</v>
       </c>
       <c r="C75" s="1">
-        <v>9.5796267729999997E-5</v>
+        <v>3.1231006579999999E-5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -6685,10 +6685,10 @@
         <v>1.4750000000000001</v>
       </c>
       <c r="B76">
-        <v>0.98686493220000004</v>
+        <v>0.99993721520000001</v>
       </c>
       <c r="C76" s="1">
-        <v>1.313506777E-2</v>
+        <v>6.2784832089999998E-5</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -6696,10 +6696,10 @@
         <v>1.476</v>
       </c>
       <c r="B77">
-        <v>0.99989175109999995</v>
+        <v>0.99968384229999996</v>
       </c>
       <c r="C77" s="1">
-        <v>1.0824894640000001E-4</v>
+        <v>3.1615771569999999E-4</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -6707,10 +6707,10 @@
         <v>1.4770000000000001</v>
       </c>
       <c r="B78">
-        <v>0.99996009350000004</v>
+        <v>0.99996900850000003</v>
       </c>
       <c r="C78" s="1">
-        <v>3.9906541720000001E-5</v>
+        <v>3.0991512489999997E-5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -6718,10 +6718,10 @@
         <v>1.478</v>
       </c>
       <c r="B79">
-        <v>0.99994124350000002</v>
+        <v>0.99994990969999997</v>
       </c>
       <c r="C79" s="1">
-        <v>5.8756486689999999E-5</v>
+        <v>5.009031488E-5</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -6729,10 +6729,10 @@
         <v>1.4790000000000001</v>
       </c>
       <c r="B80">
-        <v>0.99352246980000003</v>
+        <v>0.99145705679999996</v>
       </c>
       <c r="C80" s="1">
-        <v>6.4775301570000002E-3</v>
+        <v>8.5429432069999995E-3</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -6740,10 +6740,10 @@
         <v>1.48</v>
       </c>
       <c r="B81">
-        <v>0.99993166779999998</v>
+        <v>0.99995524199999997</v>
       </c>
       <c r="C81" s="1">
-        <v>6.8332177250000006E-5</v>
+        <v>4.4758037769999999E-5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -6751,10 +6751,10 @@
         <v>1.4810000000000001</v>
       </c>
       <c r="B82">
-        <v>0.99995863200000001</v>
+        <v>0.99996984799999999</v>
       </c>
       <c r="C82" s="1">
-        <v>4.1367956700000002E-5</v>
+        <v>3.015198024E-5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -6762,10 +6762,10 @@
         <v>1.482</v>
       </c>
       <c r="B83">
-        <v>0.99944949370000002</v>
+        <v>0.99990540949999995</v>
       </c>
       <c r="C83" s="1">
-        <v>5.5050625099999995E-4</v>
+        <v>9.4590549470000004E-5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -6773,10 +6773,10 @@
         <v>1.4830000000000001</v>
       </c>
       <c r="B84">
-        <v>0.99992962110000005</v>
+        <v>0.99888319069999998</v>
       </c>
       <c r="C84" s="1">
-        <v>7.0378924260000006E-5</v>
+        <v>1.1168092549999999E-3</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -6784,10 +6784,10 @@
         <v>1.484</v>
       </c>
       <c r="B85">
-        <v>0.99995377259999996</v>
+        <v>0.9999499731</v>
       </c>
       <c r="C85" s="1">
-        <v>4.6227376790000001E-5</v>
+        <v>5.0026854559999998E-5</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -6795,10 +6795,10 @@
         <v>1.4850000000000001</v>
       </c>
       <c r="B86">
-        <v>0.99066593830000005</v>
+        <v>0.99997091989999998</v>
       </c>
       <c r="C86" s="1">
-        <v>9.3340617389999995E-3</v>
+        <v>2.9080068230000001E-5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -6806,10 +6806,10 @@
         <v>1.486</v>
       </c>
       <c r="B87">
-        <v>0.99995919779999998</v>
+        <v>0.99995922820000005</v>
       </c>
       <c r="C87" s="1">
-        <v>4.080221217E-5</v>
+        <v>4.0771793000000002E-5</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -6817,10 +6817,10 @@
         <v>1.4870000000000001</v>
       </c>
       <c r="B88">
-        <v>0.99981659590000005</v>
+        <v>0.99983338629999996</v>
       </c>
       <c r="C88" s="1">
-        <v>1.8340414600000001E-4</v>
+        <v>1.6661366800000001E-4</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -6828,10 +6828,10 @@
         <v>1.488</v>
       </c>
       <c r="B89">
-        <v>0.99993839920000005</v>
+        <v>0.99721010450000003</v>
       </c>
       <c r="C89" s="1">
-        <v>6.1600821439999998E-5</v>
+        <v>2.7898955029999999E-3</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -6839,10 +6839,10 @@
         <v>1.4890000000000001</v>
       </c>
       <c r="B90">
-        <v>0.99992293809999999</v>
+        <v>0.99990641940000002</v>
       </c>
       <c r="C90" s="1">
-        <v>7.7061856030000004E-5</v>
+        <v>9.358058997E-5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -6850,10 +6850,10 @@
         <v>1.49</v>
       </c>
       <c r="B91">
-        <v>0.99991087670000001</v>
+        <v>0.99996075309999999</v>
       </c>
       <c r="C91" s="1">
-        <v>8.9123311180000001E-5</v>
+        <v>3.9246859139999997E-5</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -6861,10 +6861,10 @@
         <v>1.4910000000000001</v>
       </c>
       <c r="B92">
-        <v>0.99993363189999995</v>
+        <v>0.99997044700000004</v>
       </c>
       <c r="C92" s="1">
-        <v>6.6368127200000003E-5</v>
+        <v>2.9552976190000001E-5</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -6872,10 +6872,10 @@
         <v>1.492</v>
       </c>
       <c r="B93">
-        <v>0.99991710739999995</v>
+        <v>0.99996950240000004</v>
       </c>
       <c r="C93" s="1">
-        <v>8.2892625919999999E-5</v>
+        <v>3.0497586009999999E-5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -6883,10 +6883,10 @@
         <v>1.4930000000000001</v>
       </c>
       <c r="B94">
-        <v>0.99991143790000003</v>
+        <v>0.99996065619999996</v>
       </c>
       <c r="C94" s="1">
-        <v>8.8562148310000006E-5</v>
+        <v>3.9343785740000001E-5</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -6894,10 +6894,10 @@
         <v>1.494</v>
       </c>
       <c r="B95">
-        <v>0.99994621019999996</v>
+        <v>0.99993874289999995</v>
       </c>
       <c r="C95" s="1">
-        <v>5.378976086E-5</v>
+        <v>6.125708129E-5</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -6905,10 +6905,10 @@
         <v>1.4950000000000001</v>
       </c>
       <c r="B96">
-        <v>0.99966765909999999</v>
+        <v>0.99988535460000005</v>
       </c>
       <c r="C96" s="1">
-        <v>3.3234086359999998E-4</v>
+        <v>1.146454167E-4</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -6916,10 +6916,10 @@
         <v>1.496</v>
       </c>
       <c r="B97">
-        <v>0.99996117100000004</v>
+        <v>0.99973516890000003</v>
       </c>
       <c r="C97" s="1">
-        <v>3.8829012670000002E-5</v>
+        <v>2.6483108060000002E-4</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -6927,10 +6927,10 @@
         <v>1.4970000000000001</v>
       </c>
       <c r="B98">
-        <v>0.99938248399999996</v>
+        <v>0.99918508019999996</v>
       </c>
       <c r="C98" s="1">
-        <v>6.1751595630000003E-4</v>
+        <v>8.1491981630000003E-4</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -6938,10 +6938,10 @@
         <v>1.498</v>
       </c>
       <c r="B99">
-        <v>0.99994051989999999</v>
+        <v>0.99594799990000005</v>
       </c>
       <c r="C99" s="1">
-        <v>5.94801035E-5</v>
+        <v>4.0520000779999997E-3</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -6949,10 +6949,10 @@
         <v>1.4990000000000001</v>
       </c>
       <c r="B100">
-        <v>0.99995017320000001</v>
+        <v>0.94499560370000002</v>
       </c>
       <c r="C100" s="1">
-        <v>4.9826769390000001E-5</v>
+        <v>5.5004396259999998E-2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -6960,10 +6960,10 @@
         <v>1.5</v>
       </c>
       <c r="B101">
-        <v>0.57150331489999995</v>
+        <v>0.65808237390000002</v>
       </c>
       <c r="C101" s="1">
-        <v>0.4284966851</v>
+        <v>0.34191762609999998</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -6971,10 +6971,10 @@
         <v>1.5009999999999999</v>
       </c>
       <c r="B102">
-        <v>0.99994686870000005</v>
+        <v>0.94487242869999999</v>
       </c>
       <c r="C102" s="1">
-        <v>5.3131317670000002E-5</v>
+        <v>5.5127571290000003E-2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -6982,10 +6982,10 @@
         <v>1.502</v>
       </c>
       <c r="B103">
-        <v>0.99995406050000002</v>
+        <v>0.99592664109999995</v>
       </c>
       <c r="C103" s="1">
-        <v>4.593946118E-5</v>
+        <v>4.0733589030000003E-3</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -6993,10 +6993,10 @@
         <v>1.5029999999999999</v>
       </c>
       <c r="B104">
-        <v>0.99937763820000003</v>
+        <v>0.99917862999999996</v>
       </c>
       <c r="C104" s="1">
-        <v>6.2236176299999997E-4</v>
+        <v>8.213699631E-4</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -7004,10 +7004,10 @@
         <v>1.504</v>
       </c>
       <c r="B105">
-        <v>0.99987996980000005</v>
+        <v>0.99973244110000004</v>
       </c>
       <c r="C105" s="1">
-        <v>1.200302451E-4</v>
+        <v>2.675589033E-4</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -7015,10 +7015,10 @@
         <v>1.5049999999999999</v>
       </c>
       <c r="B106">
-        <v>0.99996023020000002</v>
+        <v>0.99988396310000005</v>
       </c>
       <c r="C106" s="1">
-        <v>3.9769848569999998E-5</v>
+        <v>1.16036857E-4</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -7026,10 +7026,10 @@
         <v>1.506</v>
       </c>
       <c r="B107">
-        <v>0.99994566080000002</v>
+        <v>0.99993795399999996</v>
       </c>
       <c r="C107" s="1">
-        <v>5.4339213339999999E-5</v>
+        <v>6.2045982289999998E-5</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -7037,10 +7037,10 @@
         <v>1.5069999999999999</v>
       </c>
       <c r="B108">
-        <v>0.99959974200000001</v>
+        <v>0.99996019979999995</v>
       </c>
       <c r="C108" s="1">
-        <v>4.0025799429999997E-4</v>
+        <v>3.9800154720000001E-5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -7048,10 +7048,10 @@
         <v>1.508</v>
       </c>
       <c r="B109">
-        <v>0.99960430280000001</v>
+        <v>0.99996929879999996</v>
       </c>
       <c r="C109" s="1">
-        <v>3.9569715030000001E-4</v>
+        <v>3.070122954E-5</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -7059,10 +7059,10 @@
         <v>1.5089999999999999</v>
       </c>
       <c r="B110">
-        <v>0.99993653689999995</v>
+        <v>0.99997059749999995</v>
       </c>
       <c r="C110" s="1">
-        <v>6.3463143110000005E-5</v>
+        <v>2.9402468980000001E-5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -7070,10 +7070,10 @@
         <v>1.51</v>
       </c>
       <c r="B111">
-        <v>0.99996044139999996</v>
+        <v>0.99996199149999998</v>
       </c>
       <c r="C111" s="1">
-        <v>3.9558598330000003E-5</v>
+        <v>3.8008530950000003E-5</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -7081,10 +7081,10 @@
         <v>1.5109999999999999</v>
       </c>
       <c r="B112">
-        <v>0.9999574309</v>
+        <v>0.99991589240000001</v>
       </c>
       <c r="C112" s="1">
-        <v>4.2569108459999999E-5</v>
+        <v>8.4107563829999995E-5</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -7092,10 +7092,10 @@
         <v>1.512</v>
       </c>
       <c r="B113">
-        <v>0.99993150590000002</v>
+        <v>0.99870873719999997</v>
       </c>
       <c r="C113" s="1">
-        <v>6.8494124189999998E-5</v>
+        <v>1.291262836E-3</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -7103,10 +7103,10 @@
         <v>1.5129999999999999</v>
       </c>
       <c r="B114">
-        <v>0.99982656749999999</v>
+        <v>0.99977693150000002</v>
       </c>
       <c r="C114" s="1">
-        <v>1.7343253359999999E-4</v>
+        <v>2.230684732E-4</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -7114,10 +7114,10 @@
         <v>1.514</v>
       </c>
       <c r="B115">
-        <v>0.99888925210000001</v>
+        <v>0.99995467189999998</v>
       </c>
       <c r="C115" s="1">
-        <v>1.1107479070000001E-3</v>
+        <v>4.532807493E-5</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -7125,10 +7125,10 @@
         <v>1.5149999999999999</v>
       </c>
       <c r="B116">
-        <v>0.99029413249999998</v>
+        <v>0.99997092249999997</v>
       </c>
       <c r="C116" s="1">
-        <v>9.7058675489999999E-3</v>
+        <v>2.90775035E-5</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -7136,10 +7136,10 @@
         <v>1.516</v>
       </c>
       <c r="B117">
-        <v>0.99940634719999999</v>
+        <v>0.99995793249999998</v>
       </c>
       <c r="C117" s="1">
-        <v>5.9365283949999997E-4</v>
+        <v>4.206754673E-5</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -7147,10 +7147,10 @@
         <v>1.5169999999999999</v>
       </c>
       <c r="B118">
-        <v>0.99974394109999998</v>
+        <v>0.99966662399999995</v>
       </c>
       <c r="C118" s="1">
-        <v>2.5605885190000001E-4</v>
+        <v>3.3337604589999997E-4</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -7158,10 +7158,10 @@
         <v>1.518</v>
       </c>
       <c r="B119">
-        <v>0.99982276569999995</v>
+        <v>0.99982840449999999</v>
       </c>
       <c r="C119" s="1">
-        <v>1.7723428050000001E-4</v>
+        <v>1.7159553780000001E-4</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -7169,10 +7169,10 @@
         <v>1.5189999999999999</v>
       </c>
       <c r="B120">
-        <v>0.99984274829999997</v>
+        <v>0.99996618299999995</v>
       </c>
       <c r="C120" s="1">
-        <v>1.572517208E-4</v>
+        <v>3.3816966850000001E-5</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -7180,10 +7180,10 @@
         <v>1.52</v>
       </c>
       <c r="B121">
-        <v>0.99983039819999997</v>
+        <v>0.99996544750000005</v>
       </c>
       <c r="C121" s="1">
-        <v>1.6960184250000001E-4</v>
+        <v>3.4552549430000002E-5</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -7191,10 +7191,10 @@
         <v>1.5209999999999999</v>
       </c>
       <c r="B122">
-        <v>0.99977044449999997</v>
+        <v>0.99970198539999999</v>
       </c>
       <c r="C122" s="1">
-        <v>2.2955551850000001E-4</v>
+        <v>2.9801462560000001E-4</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -7202,10 +7202,10 @@
         <v>1.522</v>
       </c>
       <c r="B123">
-        <v>0.99954047619999997</v>
+        <v>0.99989956030000005</v>
       </c>
       <c r="C123" s="1">
-        <v>4.595237992E-4</v>
+        <v>1.004397467E-4</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -7213,10 +7213,10 @@
         <v>1.5229999999999999</v>
       </c>
       <c r="B124">
-        <v>0.99691584840000003</v>
+        <v>0.99997078340000001</v>
       </c>
       <c r="C124" s="1">
-        <v>3.0841516299999999E-3</v>
+        <v>2.921657398E-5</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -7224,10 +7224,10 @@
         <v>1.524</v>
       </c>
       <c r="B125">
-        <v>0.9974927039</v>
+        <v>0.99992918760000005</v>
       </c>
       <c r="C125" s="1">
-        <v>2.5072960509999998E-3</v>
+        <v>7.0812437879999999E-5</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -7235,10 +7235,10 @@
         <v>1.5249999999999999</v>
       </c>
       <c r="B126">
-        <v>0.99976055789999996</v>
+        <v>0.9996887927</v>
       </c>
       <c r="C126" s="1">
-        <v>2.3944214650000001E-4</v>
+        <v>3.1120733409999998E-4</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -7246,10 +7246,10 @@
         <v>1.526</v>
       </c>
       <c r="B127">
-        <v>0.99991779179999996</v>
+        <v>0.99996954220000001</v>
       </c>
       <c r="C127" s="1">
-        <v>8.22081809E-5</v>
+        <v>3.0457844179999999E-5</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -7257,10 +7257,10 @@
         <v>1.5269999999999999</v>
       </c>
       <c r="B128">
-        <v>0.99995362300000001</v>
+        <v>0.99993199779999997</v>
       </c>
       <c r="C128" s="1">
-        <v>4.637698821E-5</v>
+        <v>6.8002183890000006E-5</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -7268,10 +7268,10 @@
         <v>1.528</v>
       </c>
       <c r="B129">
-        <v>0.9999613678</v>
+        <v>0.99981968619999995</v>
       </c>
       <c r="C129" s="1">
-        <v>3.8632215389999997E-5</v>
+        <v>1.803138484E-4</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -7279,10 +7279,10 @@
         <v>1.5289999999999999</v>
       </c>
       <c r="B130">
-        <v>0.9999485186</v>
+        <v>0.99997098520000005</v>
       </c>
       <c r="C130" s="1">
-        <v>5.1481385129999998E-5</v>
+        <v>2.901478644E-5</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -7290,10 +7290,10 @@
         <v>1.53</v>
       </c>
       <c r="B131">
-        <v>0.99982834939999998</v>
+        <v>0.99977931330000003</v>
       </c>
       <c r="C131" s="1">
-        <v>1.7165058499999999E-4</v>
+        <v>2.2068671679999999E-4</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -7301,10 +7301,10 @@
         <v>1.5309999999999999</v>
       </c>
       <c r="B132">
-        <v>0.99699477079999999</v>
+        <v>0.99995050429999999</v>
       </c>
       <c r="C132" s="1">
-        <v>3.0052292049999999E-3</v>
+        <v>4.9495703120000001E-5</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -7312,10 +7312,10 @@
         <v>1.532</v>
       </c>
       <c r="B133">
-        <v>0.99992075130000002</v>
+        <v>0.99995872330000002</v>
       </c>
       <c r="C133" s="1">
-        <v>7.9248652110000003E-5</v>
+        <v>4.1276718580000003E-5</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -7323,10 +7323,10 @@
         <v>1.5329999999999999</v>
       </c>
       <c r="B134">
-        <v>0.99996108459999999</v>
+        <v>0.99971906030000002</v>
       </c>
       <c r="C134" s="1">
-        <v>3.8915431740000002E-5</v>
+        <v>2.8093972549999999E-4</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -7334,10 +7334,10 @@
         <v>1.534</v>
       </c>
       <c r="B135">
-        <v>0.99993692850000004</v>
+        <v>0.99997061700000001</v>
       </c>
       <c r="C135" s="1">
-        <v>6.3071473739999994E-5</v>
+        <v>2.9383041240000001E-5</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -7345,10 +7345,10 @@
         <v>1.5349999999999999</v>
       </c>
       <c r="B136">
-        <v>0.99433581999999998</v>
+        <v>0.99252126110000005</v>
       </c>
       <c r="C136" s="1">
-        <v>5.6641800080000004E-3</v>
+        <v>7.478738853E-3</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -7356,10 +7356,10 @@
         <v>1.536</v>
       </c>
       <c r="B137">
-        <v>0.99992301920000004</v>
+        <v>0.99996984639999997</v>
       </c>
       <c r="C137" s="1">
-        <v>7.6980817890000001E-5</v>
+        <v>3.0153557780000001E-5</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -7367,10 +7367,10 @@
         <v>1.5369999999999999</v>
       </c>
       <c r="B138">
-        <v>0.99996069499999996</v>
+        <v>0.99965340189999996</v>
       </c>
       <c r="C138" s="1">
-        <v>3.9304988819999997E-5</v>
+        <v>3.4659812839999999E-4</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -7378,10 +7378,10 @@
         <v>1.538</v>
       </c>
       <c r="B139">
-        <v>0.99980952609999996</v>
+        <v>0.99996716699999999</v>
       </c>
       <c r="C139" s="1">
-        <v>1.904738684E-4</v>
+        <v>3.2833021240000002E-5</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -7389,10 +7389,10 @@
         <v>1.5389999999999999</v>
       </c>
       <c r="B140">
-        <v>0.99986259430000002</v>
+        <v>0.99977683319999999</v>
       </c>
       <c r="C140" s="1">
-        <v>1.3740569449999999E-4</v>
+        <v>2.231668349E-4</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -7400,10 +7400,10 @@
         <v>1.54</v>
       </c>
       <c r="B141">
-        <v>0.99996124710000001</v>
+        <v>0.99996722589999998</v>
       </c>
       <c r="C141" s="1">
-        <v>3.8752937859999999E-5</v>
+        <v>3.2774086589999997E-5</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -7411,10 +7411,10 @@
         <v>1.5409999999999999</v>
       </c>
       <c r="B142">
-        <v>0.99972547810000001</v>
+        <v>0.99964199769999995</v>
       </c>
       <c r="C142" s="1">
-        <v>2.7452194129999998E-4</v>
+        <v>3.5800225010000001E-4</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -7422,10 +7422,10 @@
         <v>1.542</v>
       </c>
       <c r="B143">
-        <v>0.9999244008</v>
+        <v>0.99996992669999996</v>
       </c>
       <c r="C143" s="1">
-        <v>7.5599163030000001E-5</v>
+        <v>3.0073287269999999E-5</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -7433,10 +7433,10 @@
         <v>1.5429999999999999</v>
       </c>
       <c r="B144">
-        <v>0.99995229809999997</v>
+        <v>0.99001765730000002</v>
       </c>
       <c r="C144" s="1">
-        <v>4.770191941E-5</v>
+        <v>9.9823426950000002E-3</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -7444,10 +7444,10 @@
         <v>1.544</v>
       </c>
       <c r="B145">
-        <v>0.99854328469999998</v>
+        <v>0.99997055199999996</v>
       </c>
       <c r="C145" s="1">
-        <v>1.4567152800000001E-3</v>
+        <v>2.9448030789999998E-5</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -7455,10 +7455,10 @@
         <v>1.5449999999999999</v>
       </c>
       <c r="B146">
-        <v>0.99996116719999995</v>
+        <v>0.99973442639999999</v>
       </c>
       <c r="C146" s="1">
-        <v>3.8832843970000003E-5</v>
+        <v>2.6557358840000002E-4</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -7466,10 +7466,10 @@
         <v>1.546</v>
       </c>
       <c r="B147">
-        <v>0.99943753319999995</v>
+        <v>0.99995823409999995</v>
       </c>
       <c r="C147" s="1">
-        <v>5.6246680240000003E-4</v>
+        <v>4.176590091E-5</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -7477,10 +7477,10 @@
         <v>1.5469999999999999</v>
       </c>
       <c r="B148">
-        <v>0.99995449030000005</v>
+        <v>0.99995109859999998</v>
       </c>
       <c r="C148" s="1">
-        <v>4.5509734060000001E-5</v>
+        <v>4.8901400300000001E-5</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -7488,10 +7488,10 @@
         <v>1.548</v>
       </c>
       <c r="B149">
-        <v>0.99982462729999999</v>
+        <v>0.99977433849999997</v>
       </c>
       <c r="C149" s="1">
-        <v>1.7537272560000001E-4</v>
+        <v>2.2566153869999999E-4</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -7499,10 +7499,10 @@
         <v>1.5489999999999999</v>
       </c>
       <c r="B150">
-        <v>0.99994867939999998</v>
+        <v>0.99997098520000005</v>
       </c>
       <c r="C150" s="1">
-        <v>5.1320573069999999E-5</v>
+        <v>2.901478566E-5</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -7510,10 +7510,10 @@
         <v>1.55</v>
       </c>
       <c r="B151">
-        <v>0.99983686230000002</v>
+        <v>0.99981476329999996</v>
       </c>
       <c r="C151" s="1">
-        <v>1.6313768640000001E-4</v>
+        <v>1.852367077E-4</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -7521,10 +7521,10 @@
         <v>1.5509999999999999</v>
       </c>
       <c r="B152">
-        <v>0.99995286159999996</v>
+        <v>0.99993403989999996</v>
       </c>
       <c r="C152" s="1">
-        <v>4.7138380119999999E-5</v>
+        <v>6.5960127939999996E-5</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -7532,10 +7532,10 @@
         <v>1.552</v>
       </c>
       <c r="B153">
-        <v>0.99962112759999999</v>
+        <v>0.99996921790000004</v>
       </c>
       <c r="C153" s="1">
-        <v>3.7887237270000003E-4</v>
+        <v>3.0782116049999997E-5</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -7543,10 +7543,10 @@
         <v>1.5529999999999999</v>
       </c>
       <c r="B154">
-        <v>0.99996043229999998</v>
+        <v>0.99961013840000001</v>
       </c>
       <c r="C154" s="1">
-        <v>3.9567738049999997E-5</v>
+        <v>3.898616369E-4</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -7554,10 +7554,10 @@
         <v>1.554</v>
       </c>
       <c r="B155">
-        <v>0.98980068929999998</v>
+        <v>0.99993645419999999</v>
       </c>
       <c r="C155" s="1">
-        <v>1.01993107E-2</v>
+        <v>6.3545765880000006E-5</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -7565,10 +7565,10 @@
         <v>1.5549999999999999</v>
       </c>
       <c r="B156">
-        <v>0.99995693860000001</v>
+        <v>0.99997035879999996</v>
       </c>
       <c r="C156" s="1">
-        <v>4.3061404710000003E-5</v>
+        <v>2.9641201300000001E-5</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -7576,10 +7576,10 @@
         <v>1.556</v>
       </c>
       <c r="B157">
-        <v>0.99989390909999998</v>
+        <v>0.9998671562</v>
       </c>
       <c r="C157" s="1">
-        <v>1.060908947E-4</v>
+        <v>1.3284383790000001E-4</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -7587,10 +7587,10 @@
         <v>1.5569999999999999</v>
       </c>
       <c r="B158">
-        <v>0.99986242280000004</v>
+        <v>0.99982489969999999</v>
       </c>
       <c r="C158" s="1">
-        <v>1.3757724960000001E-4</v>
+        <v>1.7510027889999999E-4</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -7598,10 +7598,10 @@
         <v>1.5580000000000001</v>
       </c>
       <c r="B159">
-        <v>0.99996063859999995</v>
+        <v>0.99996845300000003</v>
       </c>
       <c r="C159" s="1">
-        <v>3.936141365E-5</v>
+        <v>3.1547031300000001E-5</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -7609,10 +7609,10 @@
         <v>1.5589999999999999</v>
       </c>
       <c r="B160">
-        <v>0.99963125959999999</v>
+        <v>0.99996068819999995</v>
       </c>
       <c r="C160" s="1">
-        <v>3.687403763E-4</v>
+        <v>3.931182152E-5</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -7620,10 +7620,10 @@
         <v>1.56</v>
       </c>
       <c r="B161">
-        <v>0.99991250210000004</v>
+        <v>0.99949786799999996</v>
       </c>
       <c r="C161" s="1">
-        <v>8.7497919250000006E-5</v>
+        <v>5.0213195979999996E-4</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -7631,10 +7631,10 @@
         <v>1.5609999999999999</v>
       </c>
       <c r="B162">
-        <v>0.99996041719999995</v>
+        <v>0.99987952999999996</v>
       </c>
       <c r="C162" s="1">
-        <v>3.9582835309999997E-5</v>
+        <v>1.2047001949999999E-4</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -7642,10 +7642,10 @@
         <v>1.5620000000000001</v>
       </c>
       <c r="B163">
-        <v>0.99980398339999998</v>
+        <v>0.99996729309999999</v>
       </c>
       <c r="C163" s="1">
-        <v>1.9601663139999999E-4</v>
+        <v>3.2706878379999997E-5</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -7653,10 +7653,10 @@
         <v>1.5629999999999999</v>
       </c>
       <c r="B164">
-        <v>0.99979377729999996</v>
+        <v>0.99996750479999996</v>
       </c>
       <c r="C164" s="1">
-        <v>2.0622267300000001E-4</v>
+        <v>3.2495191780000002E-5</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -7664,10 +7664,10 @@
         <v>1.5640000000000001</v>
       </c>
       <c r="B165">
-        <v>0.99995847090000001</v>
+        <v>0.99990804950000001</v>
       </c>
       <c r="C165" s="1">
-        <v>4.1529124099999999E-5</v>
+        <v>9.1950549569999994E-5</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -7675,10 +7675,10 @@
         <v>1.5649999999999999</v>
       </c>
       <c r="B166">
-        <v>0.99994779050000004</v>
+        <v>0.84433625950000002</v>
       </c>
       <c r="C166" s="1">
-        <v>5.2209521510000001E-5</v>
+        <v>0.15566374050000001</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -7686,10 +7686,10 @@
         <v>1.5660000000000001</v>
       </c>
       <c r="B167">
-        <v>0.99948660180000004</v>
+        <v>0.99990328740000001</v>
       </c>
       <c r="C167" s="1">
-        <v>5.133981914E-4</v>
+        <v>9.6712576790000004E-5</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -7697,10 +7697,10 @@
         <v>1.5669999999999999</v>
       </c>
       <c r="B168">
-        <v>0.99978001699999997</v>
+        <v>0.99996384469999999</v>
       </c>
       <c r="C168" s="1">
-        <v>2.199829933E-4</v>
+        <v>3.6155263979999998E-5</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -7708,10 +7708,10 @@
         <v>1.5680000000000001</v>
       </c>
       <c r="B169">
-        <v>0.99995094679999996</v>
+        <v>0.99997095560000004</v>
       </c>
       <c r="C169" s="1">
-        <v>4.9053235049999998E-5</v>
+        <v>2.9044354659999999E-5</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -7719,10 +7719,10 @@
         <v>1.569</v>
       </c>
       <c r="B170">
-        <v>0.9999607439</v>
+        <v>0.99996281409999999</v>
       </c>
       <c r="C170" s="1">
-        <v>3.9256098470000002E-5</v>
+        <v>3.7185872150000003E-5</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -7730,10 +7730,10 @@
         <v>1.57</v>
       </c>
       <c r="B171">
-        <v>0.99993521490000004</v>
+        <v>0.9999232736</v>
       </c>
       <c r="C171" s="1">
-        <v>6.4785090479999995E-5</v>
+        <v>7.672638482E-5</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -7741,10 +7741,10 @@
         <v>1.571</v>
       </c>
       <c r="B172">
-        <v>0.99970333050000004</v>
+        <v>0.99961246400000003</v>
       </c>
       <c r="C172" s="1">
-        <v>2.9666945419999999E-4</v>
+        <v>3.8753598770000002E-4</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -7752,10 +7752,10 @@
         <v>1.5720000000000001</v>
       </c>
       <c r="B173">
-        <v>0.99585628079999999</v>
+        <v>0.9945178898</v>
       </c>
       <c r="C173" s="1">
-        <v>4.1437191959999998E-3</v>
+        <v>5.4821101889999998E-3</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -7763,10 +7763,10 @@
         <v>1.573</v>
       </c>
       <c r="B174">
-        <v>0.99983951029999996</v>
+        <v>0.9997942353</v>
       </c>
       <c r="C174" s="1">
-        <v>1.6048974050000001E-4</v>
+        <v>2.0576472740000001E-4</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -7774,10 +7774,10 @@
         <v>1.5740000000000001</v>
       </c>
       <c r="B175">
-        <v>0.99993497539999998</v>
+        <v>0.99992294179999996</v>
       </c>
       <c r="C175" s="1">
-        <v>6.5024635949999997E-5</v>
+        <v>7.7058176460000007E-5</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -7785,10 +7785,10 @@
         <v>1.575</v>
       </c>
       <c r="B176">
-        <v>0.99995548010000002</v>
+        <v>0.99995268169999996</v>
       </c>
       <c r="C176" s="1">
-        <v>4.4519864950000002E-5</v>
+        <v>4.7318298039999998E-5</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -7796,10 +7796,10 @@
         <v>1.5760000000000001</v>
       </c>
       <c r="B177">
-        <v>0.99996097589999999</v>
+        <v>0.99996354249999997</v>
       </c>
       <c r="C177" s="1">
-        <v>3.9024149390000002E-5</v>
+        <v>3.6457535699999998E-5</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -7807,10 +7807,10 @@
         <v>1.577</v>
       </c>
       <c r="B178">
-        <v>0.99996084689999998</v>
+        <v>0.99996815640000003</v>
       </c>
       <c r="C178" s="1">
-        <v>3.915310307E-5</v>
+        <v>3.1843615000000002E-5</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -7818,10 +7818,10 @@
         <v>1.5780000000000001</v>
       </c>
       <c r="B179">
-        <v>0.9999579072</v>
+        <v>0.99997010419999999</v>
       </c>
       <c r="C179" s="1">
-        <v>4.2092825300000001E-5</v>
+        <v>2.989579762E-5</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -7829,10 +7829,10 @@
         <v>1.579</v>
       </c>
       <c r="B180">
-        <v>0.99995378690000003</v>
+        <v>0.99997080670000005</v>
       </c>
       <c r="C180" s="1">
-        <v>4.62130988E-5</v>
+        <v>2.9193259359999999E-5</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -7840,10 +7840,10 @@
         <v>1.58</v>
       </c>
       <c r="B181">
-        <v>0.99995009619999997</v>
+        <v>0.9999709739</v>
       </c>
       <c r="C181" s="1">
-        <v>4.9903782309999997E-5</v>
+        <v>2.9026138249999999E-5</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -7851,10 +7851,10 @@
         <v>1.581</v>
       </c>
       <c r="B182">
-        <v>0.99994836330000003</v>
+        <v>0.99997098500000003</v>
       </c>
       <c r="C182" s="1">
-        <v>5.1636682540000001E-5</v>
+        <v>2.9015011769999999E-5</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -7862,10 +7862,10 @@
         <v>1.5820000000000001</v>
       </c>
       <c r="B183">
-        <v>0.99994936420000002</v>
+        <v>0.99997098240000004</v>
       </c>
       <c r="C183" s="1">
-        <v>5.0635785890000001E-5</v>
+        <v>2.9017593860000001E-5</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -7873,10 +7873,10 @@
         <v>1.583</v>
       </c>
       <c r="B184">
-        <v>0.99995263909999998</v>
+        <v>0.99997088639999998</v>
       </c>
       <c r="C184" s="1">
-        <v>4.7360860229999999E-5</v>
+        <v>2.9113634359999999E-5</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -7884,10 +7884,10 @@
         <v>1.5840000000000001</v>
       </c>
       <c r="B185">
-        <v>0.99995679429999995</v>
+        <v>0.99997039030000001</v>
       </c>
       <c r="C185" s="1">
-        <v>4.3205692569999997E-5</v>
+        <v>2.9609749110000001E-5</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -7895,10 +7895,10 @@
         <v>1.585</v>
       </c>
       <c r="B186">
-        <v>0.99996021329999996</v>
+        <v>0.99996890510000003</v>
       </c>
       <c r="C186" s="1">
-        <v>3.9786667470000001E-5</v>
+        <v>3.1094900589999999E-5</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -7906,10 +7906,10 @@
         <v>1.5860000000000001</v>
       </c>
       <c r="B187">
-        <v>0.99996134759999999</v>
+        <v>0.99996530819999996</v>
       </c>
       <c r="C187" s="1">
-        <v>3.865239457E-5</v>
+        <v>3.4691801950000002E-5</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -7917,10 +7917,10 @@
         <v>1.587</v>
       </c>
       <c r="B188">
-        <v>0.99995802280000001</v>
+        <v>0.99995700239999996</v>
       </c>
       <c r="C188" s="1">
-        <v>4.1977195429999997E-5</v>
+        <v>4.2997555740000001E-5</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -7928,10 +7928,10 @@
         <v>1.5880000000000001</v>
       </c>
       <c r="B189">
-        <v>0.99994422189999999</v>
+        <v>0.9999358988</v>
       </c>
       <c r="C189" s="1">
-        <v>5.577806606E-5</v>
+        <v>6.4101234409999998E-5</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -7939,10 +7939,10 @@
         <v>1.589</v>
       </c>
       <c r="B190">
-        <v>0.99989001970000002</v>
+        <v>0.99986192480000002</v>
       </c>
       <c r="C190" s="1">
-        <v>1.0998034610000001E-4</v>
+        <v>1.3807522419999999E-4</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -7950,10 +7950,10 @@
         <v>1.59</v>
       </c>
       <c r="B191">
-        <v>0.9993052067</v>
+        <v>0.99908223169999999</v>
       </c>
       <c r="C191" s="1">
-        <v>6.947933288E-4</v>
+        <v>9.177683069E-4</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -7961,10 +7961,10 @@
         <v>1.591</v>
       </c>
       <c r="B192">
-        <v>0.99907871859999997</v>
+        <v>0.99878095870000005</v>
       </c>
       <c r="C192" s="1">
-        <v>9.2128142779999999E-4</v>
+        <v>1.2190412749999999E-3</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -7972,10 +7972,10 @@
         <v>1.5920000000000001</v>
       </c>
       <c r="B193">
-        <v>0.99990611190000001</v>
+        <v>0.99988360320000003</v>
       </c>
       <c r="C193" s="1">
-        <v>9.3888100980000003E-5</v>
+        <v>1.163967931E-4</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -7983,10 +7983,10 @@
         <v>1.593</v>
       </c>
       <c r="B194">
-        <v>0.99995658350000005</v>
+        <v>0.99995450080000003</v>
       </c>
       <c r="C194" s="1">
-        <v>4.3416544190000001E-5</v>
+        <v>4.5499182759999997E-5</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -7994,10 +7994,10 @@
         <v>1.5940000000000001</v>
       </c>
       <c r="B195">
-        <v>0.99995904459999996</v>
+        <v>0.99996966629999995</v>
       </c>
       <c r="C195" s="1">
-        <v>4.0955429520000001E-5</v>
+        <v>3.0333700089999999E-5</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -8005,10 +8005,10 @@
         <v>1.595</v>
       </c>
       <c r="B196">
-        <v>0.99990713600000003</v>
+        <v>0.99996893229999995</v>
       </c>
       <c r="C196" s="1">
-        <v>9.2864012010000007E-5</v>
+        <v>3.1067680030000002E-5</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -8016,10 +8016,10 @@
         <v>1.5960000000000001</v>
       </c>
       <c r="B197">
-        <v>0.94071497439999996</v>
+        <v>0.99994417440000005</v>
       </c>
       <c r="C197" s="1">
-        <v>5.9285025579999998E-2</v>
+        <v>5.5825575320000002E-5</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -8027,10 +8027,10 @@
         <v>1.597</v>
       </c>
       <c r="B198">
-        <v>0.99990694270000002</v>
+        <v>0.99957004360000001</v>
       </c>
       <c r="C198" s="1">
-        <v>9.3057257139999994E-5</v>
+        <v>4.2995643059999999E-4</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -8038,10 +8038,10 @@
         <v>1.5980000000000001</v>
       </c>
       <c r="B199">
-        <v>0.99996097149999996</v>
+        <v>0.99969929930000001</v>
       </c>
       <c r="C199" s="1">
-        <v>3.9028510250000001E-5</v>
+        <v>3.0070073399999999E-4</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -8049,10 +8049,10 @@
         <v>1.599</v>
       </c>
       <c r="B200">
-        <v>0.99993301329999995</v>
+        <v>0.99995466659999999</v>
       </c>
       <c r="C200" s="1">
-        <v>6.6986719140000003E-5</v>
+        <v>4.5333362249999997E-5</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -8060,10 +8060,10 @@
         <v>1.6</v>
       </c>
       <c r="B201">
-        <v>0.57150331489999995</v>
+        <v>0.99997098520000005</v>
       </c>
       <c r="C201" s="1">
-        <v>0.4284966851</v>
+        <v>2.9014756060000001E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>